<commit_message>
Delete test.ipynb Update tests n_samples = 1000 Added test2
</commit_message>
<xml_diff>
--- a/tests/test1/d10/N, 0.0.xlsx
+++ b/tests/test1/d10/N, 0.0.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -532,13 +532,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>9.999999999998462</v>
+        <v>10.00000000000044</v>
       </c>
       <c r="G2" t="n">
-        <v>98.786430706917</v>
+        <v>98.78643070691872</v>
       </c>
       <c r="H2" t="n">
-        <v>11.58227239646679</v>
+        <v>11.5822723964697</v>
       </c>
       <c r="I2" t="n">
         <v>70.56128143157282</v>
@@ -547,16 +547,16 @@
         <v>15.80711097780685</v>
       </c>
       <c r="K2" t="n">
-        <v>70.56128143157235</v>
+        <v>70.56128143157291</v>
       </c>
       <c r="L2" t="n">
-        <v>15.80711097780371</v>
+        <v>15.80711097780725</v>
       </c>
       <c r="M2" t="n">
-        <v>3.813235278855026e-26</v>
+        <v>3.918382019510714e-27</v>
       </c>
       <c r="N2" t="n">
-        <v>9.647617397205593e-13</v>
+        <v>2.156748969569024e-13</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>0.0007229999999935899</v>
+        <v>0.0002675000000014194</v>
       </c>
     </row>
     <row r="3">
@@ -584,13 +584,13 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>9.999999999998877</v>
+        <v>10.00000000000033</v>
       </c>
       <c r="G3" t="n">
-        <v>75.06396084646215</v>
+        <v>75.06396084646357</v>
       </c>
       <c r="H3" t="n">
-        <v>11.64389392130423</v>
+        <v>11.64389392130642</v>
       </c>
       <c r="I3" t="n">
         <v>53.17592866838513</v>
@@ -599,16 +599,16 @@
         <v>18.32782196423818</v>
       </c>
       <c r="K3" t="n">
-        <v>53.17592866838478</v>
+        <v>53.1759286683852</v>
       </c>
       <c r="L3" t="n">
-        <v>18.32782196423583</v>
+        <v>18.32782196423901</v>
       </c>
       <c r="M3" t="n">
-        <v>3.296075708296818e-26</v>
+        <v>3.81254349076158e-27</v>
       </c>
       <c r="N3" t="n">
-        <v>6.868375765760203e-13</v>
+        <v>2.14676369353826e-13</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>0.0007531999999912387</v>
+        <v>0.0002551000000003967</v>
       </c>
     </row>
     <row r="4">
@@ -636,13 +636,13 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>9.999999999999982</v>
+        <v>10.00000000000009</v>
       </c>
       <c r="G4" t="n">
-        <v>78.47908238555958</v>
+        <v>78.47908238556136</v>
       </c>
       <c r="H4" t="n">
-        <v>3.311114781934739</v>
+        <v>3.31111478193473</v>
       </c>
       <c r="I4" t="n">
         <v>31.7678424560353</v>
@@ -651,16 +651,16 @@
         <v>9.618122158119826</v>
       </c>
       <c r="K4" t="n">
-        <v>31.76784245603526</v>
+        <v>31.76784245603537</v>
       </c>
       <c r="L4" t="n">
         <v>9.618122158120739</v>
       </c>
       <c r="M4" t="n">
-        <v>1.356173972387916e-27</v>
+        <v>9.243366165374418e-28</v>
       </c>
       <c r="N4" t="n">
-        <v>2.248468411363621e-13</v>
+        <v>2.224040598703054e-13</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>0.000575200000000109</v>
+        <v>0.0002408999999996553</v>
       </c>
     </row>
     <row r="5">
@@ -688,13 +688,13 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>10.00000000000255</v>
+        <v>9.999999999999732</v>
       </c>
       <c r="G5" t="n">
-        <v>99.1436224634255</v>
+        <v>99.14362246342343</v>
       </c>
       <c r="H5" t="n">
-        <v>11.49777387142107</v>
+        <v>11.49777387141685</v>
       </c>
       <c r="I5" t="n">
         <v>70.66253786388728</v>
@@ -703,16 +703,16 @@
         <v>15.67687823027242</v>
       </c>
       <c r="K5" t="n">
-        <v>70.66253786388791</v>
+        <v>70.66253786388721</v>
       </c>
       <c r="L5" t="n">
-        <v>15.67687823027711</v>
+        <v>15.67687823027198</v>
       </c>
       <c r="M5" t="n">
-        <v>1.197574230120601e-25</v>
+        <v>1.485762209162658e-27</v>
       </c>
       <c r="N5" t="n">
-        <v>1.530581022282074e-12</v>
+        <v>1.533717283904055e-13</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>0.0003268000000105076</v>
+        <v>0.0002358000000004523</v>
       </c>
     </row>
     <row r="6">
@@ -740,13 +740,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>10.0000000000022</v>
+        <v>10.0000000000014</v>
       </c>
       <c r="G6" t="n">
-        <v>174.0653710224595</v>
+        <v>174.0653710224604</v>
       </c>
       <c r="H6" t="n">
-        <v>9.566786990111407</v>
+        <v>9.566786990110417</v>
       </c>
       <c r="I6" t="n">
         <v>149.7044734839228</v>
@@ -755,16 +755,16 @@
         <v>4.673171010711503</v>
       </c>
       <c r="K6" t="n">
-        <v>149.7044734839209</v>
+        <v>149.7044734839216</v>
       </c>
       <c r="L6" t="n">
-        <v>4.673171010712607</v>
+        <v>4.67317101071214</v>
       </c>
       <c r="M6" t="n">
-        <v>5.677152223630185e-25</v>
+        <v>2.3728932100462e-25</v>
       </c>
       <c r="N6" t="n">
-        <v>1.648835644897094e-12</v>
+        <v>1.016890486098248e-12</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>0.0003469999999907714</v>
+        <v>0.000264800000000065</v>
       </c>
     </row>
     <row r="7">
@@ -792,13 +792,13 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>10.0000000000002</v>
+        <v>9.999999999998996</v>
       </c>
       <c r="G7" t="n">
-        <v>39.95877079615328</v>
+        <v>39.95877079615218</v>
       </c>
       <c r="H7" t="n">
-        <v>13.44878767412891</v>
+        <v>13.44878767412662</v>
       </c>
       <c r="I7" t="n">
         <v>30.28257116656484</v>
@@ -807,16 +807,16 @@
         <v>22.87529985576693</v>
       </c>
       <c r="K7" t="n">
-        <v>30.2825711665649</v>
+        <v>30.28257116656449</v>
       </c>
       <c r="L7" t="n">
-        <v>22.87529985576689</v>
+        <v>22.87529985576319</v>
       </c>
       <c r="M7" t="n">
-        <v>2.008777572365876e-27</v>
+        <v>4.592584220012034e-26</v>
       </c>
       <c r="N7" t="n">
-        <v>9.39670969795561e-14</v>
+        <v>7.339612845874106e-13</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>0.0003438000000102193</v>
+        <v>0.0002366999999985353</v>
       </c>
     </row>
     <row r="8">
@@ -844,13 +844,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>9.99999999999655</v>
+        <v>10.00000000000436</v>
       </c>
       <c r="G8" t="n">
-        <v>160.7148272584849</v>
+        <v>160.7148272584745</v>
       </c>
       <c r="H8" t="n">
-        <v>6.983757663610596</v>
+        <v>6.98375766361858</v>
       </c>
       <c r="I8" t="n">
         <v>97.61618025069936</v>
@@ -859,16 +859,16 @@
         <v>3.973338297383755</v>
       </c>
       <c r="K8" t="n">
-        <v>97.61618025069853</v>
+        <v>97.61618025070032</v>
       </c>
       <c r="L8" t="n">
-        <v>3.973338297381708</v>
+        <v>3.973338297386365</v>
       </c>
       <c r="M8" t="n">
-        <v>4.829941627315092e-25</v>
+        <v>7.653169216637073e-25</v>
       </c>
       <c r="N8" t="n">
-        <v>2.443028687467013e-12</v>
+        <v>3.075786487289376e-12</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>0.0004861999999974387</v>
+        <v>0.0002635000000008603</v>
       </c>
     </row>
     <row r="9">
@@ -896,13 +896,13 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>9.999999999999979</v>
+        <v>9.999999999999995</v>
       </c>
       <c r="G9" t="n">
-        <v>13.73549208731227</v>
+        <v>13.73549208731229</v>
       </c>
       <c r="H9" t="n">
-        <v>12.35902550688106</v>
+        <v>12.35902550688118</v>
       </c>
       <c r="I9" t="n">
         <v>12.15137765332865</v>
@@ -911,16 +911,16 @@
         <v>22.28974380606835</v>
       </c>
       <c r="K9" t="n">
-        <v>12.15137765332861</v>
+        <v>12.15137765332862</v>
       </c>
       <c r="L9" t="n">
-        <v>22.28974380606762</v>
+        <v>22.28974380606778</v>
       </c>
       <c r="M9" t="n">
-        <v>1.164762434707389e-27</v>
+        <v>4.618653353810803e-28</v>
       </c>
       <c r="N9" t="n">
-        <v>1.254207879678988e-13</v>
+        <v>8.904078743900638e-14</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>0.0003533000000004449</v>
+        <v>0.000197599999999909</v>
       </c>
     </row>
     <row r="10">
@@ -948,13 +948,13 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>9.999999999999785</v>
+        <v>10.00000000000321</v>
       </c>
       <c r="G10" t="n">
-        <v>157.217292502527</v>
+        <v>157.2172925025259</v>
       </c>
       <c r="H10" t="n">
-        <v>14.62248795385081</v>
+        <v>14.62248795385683</v>
       </c>
       <c r="I10" t="n">
         <v>137.8318815863209</v>
@@ -963,16 +963,16 @@
         <v>11.86534188679525</v>
       </c>
       <c r="K10" t="n">
-        <v>137.8318815863209</v>
+        <v>137.8318815863199</v>
       </c>
       <c r="L10" t="n">
-        <v>11.86534188679486</v>
+        <v>11.86534188679923</v>
       </c>
       <c r="M10" t="n">
-        <v>4.037124956563503e-27</v>
+        <v>7.324006640586341e-25</v>
       </c>
       <c r="N10" t="n">
-        <v>1.355506902057276e-13</v>
+        <v>1.790233895132588e-12</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -980,7 +980,7 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>0.0003042999999962603</v>
+        <v>0.0001986000000009369</v>
       </c>
     </row>
     <row r="11">
@@ -1000,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>10.00000000000023</v>
+        <v>9.999999999999961</v>
       </c>
       <c r="G11" t="n">
-        <v>1.867347699426128</v>
+        <v>1.867347699425874</v>
       </c>
       <c r="H11" t="n">
-        <v>9.022495105784714</v>
+        <v>9.022495105784763</v>
       </c>
       <c r="I11" t="n">
         <v>4.782971926670573</v>
@@ -1015,16 +1015,16 @@
         <v>18.26849864379155</v>
       </c>
       <c r="K11" t="n">
-        <v>4.782971926670624</v>
+        <v>4.782971926670535</v>
       </c>
       <c r="L11" t="n">
-        <v>18.26849864379163</v>
+        <v>18.26849864379143</v>
       </c>
       <c r="M11" t="n">
-        <v>6.775820313812234e-28</v>
+        <v>2.612299564546052e-28</v>
       </c>
       <c r="N11" t="n">
-        <v>6.737964172210172e-14</v>
+        <v>4.869909135363073e-14</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>0.0003375000000005457</v>
+        <v>0.0002385000000000304</v>
       </c>
     </row>
     <row r="12">
@@ -1052,13 +1052,13 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>10.00000000000043</v>
+        <v>10.00000000000042</v>
       </c>
       <c r="G12" t="n">
-        <v>138.837715788013</v>
+        <v>138.8377157880136</v>
       </c>
       <c r="H12" t="n">
-        <v>3.249023392313085</v>
+        <v>3.249023392313083</v>
       </c>
       <c r="I12" t="n">
         <v>40.03006317522596</v>
@@ -1070,13 +1070,13 @@
         <v>40.03006317522649</v>
       </c>
       <c r="L12" t="n">
-        <v>5.809547132347165</v>
+        <v>5.809547132347116</v>
       </c>
       <c r="M12" t="n">
-        <v>2.72468904039906e-26</v>
+        <v>2.554566397623417e-26</v>
       </c>
       <c r="N12" t="n">
-        <v>3.835026300022807e-13</v>
+        <v>3.527735125955172e-13</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1084,7 +1084,7 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>0.000583500000004733</v>
+        <v>0.0002732999999999208</v>
       </c>
     </row>
     <row r="13">
@@ -1104,13 +1104,13 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>10.00000000000006</v>
+        <v>9.999999999999977</v>
       </c>
       <c r="G13" t="n">
-        <v>32.44854399781889</v>
+        <v>32.4485439978188</v>
       </c>
       <c r="H13" t="n">
-        <v>3.233702897851484</v>
+        <v>3.233702897851377</v>
       </c>
       <c r="I13" t="n">
         <v>16.97012183948808</v>
@@ -1119,16 +1119,16 @@
         <v>11.14346017967418</v>
       </c>
       <c r="K13" t="n">
-        <v>16.97012183948812</v>
+        <v>16.97012183948804</v>
       </c>
       <c r="L13" t="n">
-        <v>11.14346017967401</v>
+        <v>11.14346017967381</v>
       </c>
       <c r="M13" t="n">
-        <v>2.544972256181463e-28</v>
+        <v>1.093126178607466e-27</v>
       </c>
       <c r="N13" t="n">
-        <v>5.158638796691111e-14</v>
+        <v>1.616098110185524e-13</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>0.0005931000000032327</v>
+        <v>0.0002452000000001675</v>
       </c>
     </row>
     <row r="14">
@@ -1156,13 +1156,13 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>10.0000000000006</v>
+        <v>10.00000000000024</v>
       </c>
       <c r="G14" t="n">
-        <v>27.74931162834185</v>
+        <v>27.74931162834136</v>
       </c>
       <c r="H14" t="n">
-        <v>11.88059635818568</v>
+        <v>11.88059635818518</v>
       </c>
       <c r="I14" t="n">
         <v>21.32604566380087</v>
@@ -1171,16 +1171,16 @@
         <v>21.47093508922593</v>
       </c>
       <c r="K14" t="n">
-        <v>21.32604566380112</v>
+        <v>21.32604566380097</v>
       </c>
       <c r="L14" t="n">
-        <v>21.47093508922658</v>
+        <v>21.47093508922566</v>
       </c>
       <c r="M14" t="n">
-        <v>1.274021190721444e-26</v>
+        <v>2.025205435606836e-27</v>
       </c>
       <c r="N14" t="n">
-        <v>3.071629079574054e-13</v>
+        <v>1.255639322506474e-13</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1188,7 +1188,7 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>0.0003256999999905474</v>
+        <v>0.0003390000000003113</v>
       </c>
     </row>
     <row r="15">
@@ -1208,13 +1208,13 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>10.00000000000143</v>
+        <v>9.999999999998945</v>
       </c>
       <c r="G15" t="n">
-        <v>139.9864339032864</v>
+        <v>139.9864339032884</v>
       </c>
       <c r="H15" t="n">
-        <v>5.850494640420281</v>
+        <v>5.850494640417965</v>
       </c>
       <c r="I15" t="n">
         <v>70.55697937574554</v>
@@ -1223,16 +1223,16 @@
         <v>6.028251123835125</v>
       </c>
       <c r="K15" t="n">
-        <v>70.55697937574645</v>
+        <v>70.55697937574482</v>
       </c>
       <c r="L15" t="n">
-        <v>6.028251123836329</v>
+        <v>6.028251123834295</v>
       </c>
       <c r="M15" t="n">
-        <v>1.255122751900046e-25</v>
+        <v>7.066389828069417e-26</v>
       </c>
       <c r="N15" t="n">
-        <v>1.16104789623433e-12</v>
+        <v>8.525754835752701e-13</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1240,7 +1240,7 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>0.0005282000000050857</v>
+        <v>0.0002607000000001136</v>
       </c>
     </row>
     <row r="16">
@@ -1260,13 +1260,13 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>10.0000000000007</v>
+        <v>9.99999999999855</v>
       </c>
       <c r="G16" t="n">
-        <v>92.50980187908486</v>
+        <v>92.50980187908307</v>
       </c>
       <c r="H16" t="n">
-        <v>12.27798062495265</v>
+        <v>12.27798062494929</v>
       </c>
       <c r="I16" t="n">
         <v>67.01959217131787</v>
@@ -1275,16 +1275,16 @@
         <v>17.25965100693092</v>
       </c>
       <c r="K16" t="n">
-        <v>67.01959217131805</v>
+        <v>67.0195921713175</v>
       </c>
       <c r="L16" t="n">
-        <v>17.25965100693224</v>
+        <v>17.25965100692796</v>
       </c>
       <c r="M16" t="n">
-        <v>8.423100735741541e-27</v>
+        <v>3.876898298461872e-26</v>
       </c>
       <c r="N16" t="n">
-        <v>4.065378140284111e-13</v>
+        <v>8.702338794045781e-13</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>0.0003224999999957845</v>
+        <v>0.0002379999999995164</v>
       </c>
     </row>
     <row r="17">
@@ -1312,13 +1312,13 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>9.999999999999028</v>
+        <v>9.999999999999554</v>
       </c>
       <c r="G17" t="n">
-        <v>152.7871855083459</v>
+        <v>152.7871855083453</v>
       </c>
       <c r="H17" t="n">
-        <v>5.146751099051181</v>
+        <v>5.146751099051621</v>
       </c>
       <c r="I17" t="n">
         <v>64.66687573308144</v>
@@ -1327,16 +1327,16 @@
         <v>4.419793767587765</v>
       </c>
       <c r="K17" t="n">
-        <v>64.66687573308043</v>
+        <v>64.6668757330811</v>
       </c>
       <c r="L17" t="n">
-        <v>4.419793767587001</v>
+        <v>4.41979376758732</v>
       </c>
       <c r="M17" t="n">
-        <v>1.040490362201114e-25</v>
+        <v>2.003800401095024e-26</v>
       </c>
       <c r="N17" t="n">
-        <v>9.770310530312705e-13</v>
+        <v>4.559327428321977e-13</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1344,7 +1344,7 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>0.0005503999999945108</v>
+        <v>0.0002384000000006381</v>
       </c>
     </row>
     <row r="18">
@@ -1364,13 +1364,13 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>9.999999999999833</v>
+        <v>10.00000000000014</v>
       </c>
       <c r="G18" t="n">
-        <v>40.19239424763678</v>
+        <v>40.19239424763722</v>
       </c>
       <c r="H18" t="n">
-        <v>9.277960096807867</v>
+        <v>9.277960096808263</v>
       </c>
       <c r="I18" t="n">
         <v>27.73953336539376</v>
@@ -1379,16 +1379,16 @@
         <v>17.9514684390679</v>
       </c>
       <c r="K18" t="n">
-        <v>27.73953336539369</v>
+        <v>27.73953336539383</v>
       </c>
       <c r="L18" t="n">
-        <v>17.95146843906766</v>
+        <v>17.95146843906837</v>
       </c>
       <c r="M18" t="n">
-        <v>1.928792730028744e-27</v>
+        <v>7.632223676209805e-28</v>
       </c>
       <c r="N18" t="n">
-        <v>1.149219465736615e-13</v>
+        <v>1.043009005249514e-13</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1396,7 +1396,7 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>0.0005208000000038737</v>
+        <v>0.0002088999999987351</v>
       </c>
     </row>
     <row r="19">
@@ -1416,13 +1416,13 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>10.00000000000077</v>
+        <v>9.999999999998137</v>
       </c>
       <c r="G19" t="n">
-        <v>53.03970048368086</v>
+        <v>53.03970048367671</v>
       </c>
       <c r="H19" t="n">
-        <v>9.367041067264495</v>
+        <v>9.367041067261379</v>
       </c>
       <c r="I19" t="n">
         <v>35.67338189562808</v>
@@ -1431,16 +1431,16 @@
         <v>17.4087621630154</v>
       </c>
       <c r="K19" t="n">
-        <v>35.67338189562843</v>
+        <v>35.67338189562726</v>
       </c>
       <c r="L19" t="n">
-        <v>17.40876216301645</v>
+        <v>17.40876216301099</v>
       </c>
       <c r="M19" t="n">
-        <v>2.539397555048875e-26</v>
+        <v>1.273158727901294e-25</v>
       </c>
       <c r="N19" t="n">
-        <v>4.715629952406103e-13</v>
+        <v>1.278521434316657e-12</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1448,7 +1448,7 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>0.0003337999999928343</v>
+        <v>0.000210900000000791</v>
       </c>
     </row>
     <row r="20">
@@ -1468,13 +1468,13 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>10.0000000000009</v>
+        <v>10.00000000000304</v>
       </c>
       <c r="G20" t="n">
-        <v>117.0673635131269</v>
+        <v>117.067363513128</v>
       </c>
       <c r="H20" t="n">
-        <v>9.06544048481925</v>
+        <v>9.065440484821945</v>
       </c>
       <c r="I20" t="n">
         <v>77.36702495454749</v>
@@ -1483,16 +1483,16 @@
         <v>11.12685015605182</v>
       </c>
       <c r="K20" t="n">
-        <v>77.36702495454777</v>
+        <v>77.36702495454841</v>
       </c>
       <c r="L20" t="n">
-        <v>11.12685015605329</v>
+        <v>11.12685015605612</v>
       </c>
       <c r="M20" t="n">
-        <v>1.821458693442563e-26</v>
+        <v>2.066385468415386e-25</v>
       </c>
       <c r="N20" t="n">
-        <v>6.165598985178326e-13</v>
+        <v>1.965718566444837e-12</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>0.0003128000000032216</v>
+        <v>0.0003296999999999883</v>
       </c>
     </row>
     <row r="21">
@@ -1520,13 +1520,13 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>9.99999999999995</v>
+        <v>10.00000000000028</v>
       </c>
       <c r="G21" t="n">
-        <v>17.55604831490122</v>
+        <v>17.55604831490163</v>
       </c>
       <c r="H21" t="n">
-        <v>12.13499660009819</v>
+        <v>12.13499660009884</v>
       </c>
       <c r="I21" t="n">
         <v>14.65846372863805</v>
@@ -1535,16 +1535,16 @@
         <v>21.98288036784542</v>
       </c>
       <c r="K21" t="n">
-        <v>14.65846372863803</v>
+        <v>14.65846372863819</v>
       </c>
       <c r="L21" t="n">
-        <v>21.98288036784436</v>
+        <v>21.98288036784546</v>
       </c>
       <c r="M21" t="n">
-        <v>1.739737648140979e-28</v>
+        <v>5.097754480133218e-27</v>
       </c>
       <c r="N21" t="n">
-        <v>1.079967148630251e-13</v>
+        <v>1.632182591403014e-13</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>0.0003177000000107455</v>
+        <v>0.0002461000000000269</v>
       </c>
     </row>
     <row r="22">
@@ -1572,13 +1572,13 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>10.000000000001</v>
+        <v>10.00000000000364</v>
       </c>
       <c r="G22" t="n">
-        <v>105.8635441939099</v>
+        <v>105.8635441939115</v>
       </c>
       <c r="H22" t="n">
-        <v>13.77256473491476</v>
+        <v>13.77256473491928</v>
       </c>
       <c r="I22" t="n">
         <v>80.46804950751098</v>
@@ -1587,16 +1587,16 @@
         <v>17.3070565800005</v>
       </c>
       <c r="K22" t="n">
-        <v>80.46804950751114</v>
+        <v>80.46804950751162</v>
       </c>
       <c r="L22" t="n">
-        <v>17.30705658000229</v>
+        <v>17.30705658000742</v>
       </c>
       <c r="M22" t="n">
-        <v>1.350874471628268e-26</v>
+        <v>1.512860146312806e-25</v>
       </c>
       <c r="N22" t="n">
-        <v>5.454618476898233e-13</v>
+        <v>2.013333905316851e-12</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1604,7 +1604,7 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>0.0003260000000011587</v>
+        <v>0.0001920999999995843</v>
       </c>
     </row>
     <row r="23">
@@ -1624,13 +1624,13 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>9.999999999999934</v>
+        <v>10.00000000000002</v>
       </c>
       <c r="G23" t="n">
-        <v>8.770478545642726</v>
+        <v>8.770478545642955</v>
       </c>
       <c r="H23" t="n">
-        <v>6.469315917477708</v>
+        <v>6.469315917477803</v>
       </c>
       <c r="I23" t="n">
         <v>8.886792062587165</v>
@@ -1639,16 +1639,16 @@
         <v>15.23897862130467</v>
       </c>
       <c r="K23" t="n">
-        <v>8.886792062587102</v>
+        <v>8.886792062587165</v>
       </c>
       <c r="L23" t="n">
-        <v>15.23897862130468</v>
+        <v>15.23897862130489</v>
       </c>
       <c r="M23" t="n">
-        <v>5.321550453137111e-28</v>
+        <v>6.059457752813007e-29</v>
       </c>
       <c r="N23" t="n">
-        <v>5.712097330577144e-14</v>
+        <v>2.546620033398204e-14</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1656,7 +1656,7 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>0.0003329000000036331</v>
+        <v>0.0001986000000009369</v>
       </c>
     </row>
     <row r="24">
@@ -1676,13 +1676,13 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>9.999999999999911</v>
+        <v>9.999999999999808</v>
       </c>
       <c r="G24" t="n">
-        <v>37.52289672459162</v>
+        <v>37.52289672459166</v>
       </c>
       <c r="H24" t="n">
-        <v>8.780172741160232</v>
+        <v>8.780172741159957</v>
       </c>
       <c r="I24" t="n">
         <v>25.73745290239647</v>
@@ -1691,16 +1691,16 @@
         <v>17.47349577797121</v>
       </c>
       <c r="K24" t="n">
-        <v>25.73745290239644</v>
+        <v>25.73745290239639</v>
       </c>
       <c r="L24" t="n">
-        <v>17.47349577797122</v>
+        <v>17.4734957779708</v>
       </c>
       <c r="M24" t="n">
-        <v>8.547875069968217e-28</v>
+        <v>6.634432966246597e-27</v>
       </c>
       <c r="N24" t="n">
-        <v>5.421923762497394e-14</v>
+        <v>1.840367286473773e-13</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>0.0003312999999991462</v>
+        <v>0.0002151000000001346</v>
       </c>
     </row>
     <row r="25">
@@ -1728,13 +1728,13 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>10.0000000000019</v>
+        <v>9.999999999997243</v>
       </c>
       <c r="G25" t="n">
-        <v>93.11361909238752</v>
+        <v>93.11361909238401</v>
       </c>
       <c r="H25" t="n">
-        <v>14.3635512457811</v>
+        <v>14.36355124577289</v>
       </c>
       <c r="I25" t="n">
         <v>70.67112797219256</v>
@@ -1743,16 +1743,16 @@
         <v>19.47923218856673</v>
       </c>
       <c r="K25" t="n">
-        <v>70.67112797219298</v>
+        <v>70.671127972192</v>
       </c>
       <c r="L25" t="n">
-        <v>19.47923218857153</v>
+        <v>19.47923218856129</v>
       </c>
       <c r="M25" t="n">
-        <v>4.580416492207844e-26</v>
+        <v>1.026098813401642e-25</v>
       </c>
       <c r="N25" t="n">
-        <v>1.126183866915102e-12</v>
+        <v>1.507345789781534e-12</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -1760,7 +1760,7 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>0.0004895999999945388</v>
+        <v>0.000255499999999742</v>
       </c>
     </row>
     <row r="26">
@@ -1780,13 +1780,13 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>10.00000000000096</v>
+        <v>10.00000000000491</v>
       </c>
       <c r="G26" t="n">
-        <v>172.8031146004646</v>
+        <v>172.8031146004616</v>
       </c>
       <c r="H26" t="n">
-        <v>11.39414459939626</v>
+        <v>11.39414459940181</v>
       </c>
       <c r="I26" t="n">
         <v>154.9934456744326</v>
@@ -1795,16 +1795,16 @@
         <v>6.82101990562933</v>
       </c>
       <c r="K26" t="n">
-        <v>154.9934456744319</v>
+        <v>154.9934456744293</v>
       </c>
       <c r="L26" t="n">
-        <v>6.821019905630278</v>
+        <v>6.821019905633265</v>
       </c>
       <c r="M26" t="n">
-        <v>1.483132149729578e-25</v>
+        <v>3.935333217543218e-24</v>
       </c>
       <c r="N26" t="n">
-        <v>7.156070097538253e-13</v>
+        <v>3.400322262377801e-12</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>0.0003451999999981581</v>
+        <v>0.0002118999999982663</v>
       </c>
     </row>
     <row r="27">
@@ -1832,13 +1832,13 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>10.00000000001132</v>
+        <v>10.00000000000646</v>
       </c>
       <c r="G27" t="n">
-        <v>156.6223445928922</v>
+        <v>156.6223445928948</v>
       </c>
       <c r="H27" t="n">
-        <v>9.987323144085735</v>
+        <v>9.987323144079284</v>
       </c>
       <c r="I27" t="n">
         <v>121.4009088187373</v>
@@ -1847,16 +1847,16 @@
         <v>6.942709063967283</v>
       </c>
       <c r="K27" t="n">
-        <v>121.400908818735</v>
+        <v>121.400908818736</v>
       </c>
       <c r="L27" t="n">
-        <v>6.942709063976849</v>
+        <v>6.942709063972754</v>
       </c>
       <c r="M27" t="n">
-        <v>3.408052983176136e-24</v>
+        <v>1.105639437375364e-24</v>
       </c>
       <c r="N27" t="n">
-        <v>6.77187324706419e-12</v>
+        <v>3.868931669459529e-12</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         </is>
       </c>
       <c r="P27" t="n">
-        <v>0.0003341000000034455</v>
+        <v>0.0001931000000006122</v>
       </c>
     </row>
     <row r="28">
@@ -1884,13 +1884,13 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>9.999999999999986</v>
+        <v>9.999999999999838</v>
       </c>
       <c r="G28" t="n">
-        <v>55.42829147249473</v>
+        <v>55.4282914724947</v>
       </c>
       <c r="H28" t="n">
-        <v>9.232697751663586</v>
+        <v>9.232697751663331</v>
       </c>
       <c r="I28" t="n">
         <v>36.9783150738388</v>
@@ -1899,16 +1899,16 @@
         <v>17.11232764246076</v>
       </c>
       <c r="K28" t="n">
-        <v>36.97831507383879</v>
+        <v>36.97831507383874</v>
       </c>
       <c r="L28" t="n">
-        <v>17.11232764246036</v>
+        <v>17.11232764245996</v>
       </c>
       <c r="M28" t="n">
-        <v>4.302215004497235e-29</v>
+        <v>2.761362225265252e-27</v>
       </c>
       <c r="N28" t="n">
-        <v>4.489059886322495e-14</v>
+        <v>1.688676203693788e-13</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1916,7 +1916,7 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>0.0005436999999943737</v>
+        <v>0.0001977000000010776</v>
       </c>
     </row>
     <row r="29">
@@ -1936,13 +1936,13 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>10.00000000000005</v>
+        <v>10.00000000000235</v>
       </c>
       <c r="G29" t="n">
-        <v>76.62985389340147</v>
+        <v>76.62985389340344</v>
       </c>
       <c r="H29" t="n">
-        <v>12.77500488593464</v>
+        <v>12.77500488593842</v>
       </c>
       <c r="I29" t="n">
         <v>55.80674075854401</v>
@@ -1951,16 +1951,16 @@
         <v>19.44632462639266</v>
       </c>
       <c r="K29" t="n">
-        <v>55.80674075854404</v>
+        <v>55.80674075854465</v>
       </c>
       <c r="L29" t="n">
-        <v>19.44632462639234</v>
+        <v>19.44632462639768</v>
       </c>
       <c r="M29" t="n">
-        <v>1.131435417066918e-27</v>
+        <v>1.284902630299329e-25</v>
       </c>
       <c r="N29" t="n">
-        <v>4.197502000672423e-14</v>
+        <v>1.382711791890043e-12</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         </is>
       </c>
       <c r="P29" t="n">
-        <v>0.000325399999994147</v>
+        <v>0.000188299999999586</v>
       </c>
     </row>
     <row r="30">
@@ -1988,13 +1988,13 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>10.00000000000092</v>
+        <v>9.999999999998842</v>
       </c>
       <c r="G30" t="n">
-        <v>131.2224736120415</v>
+        <v>131.2224736120413</v>
       </c>
       <c r="H30" t="n">
-        <v>9.734875227932912</v>
+        <v>9.734875227930148</v>
       </c>
       <c r="I30" t="n">
         <v>91.80924814573706</v>
@@ -2003,16 +2003,16 @@
         <v>9.961999912823932</v>
       </c>
       <c r="K30" t="n">
-        <v>91.80924814573726</v>
+        <v>91.80924814573685</v>
       </c>
       <c r="L30" t="n">
-        <v>9.961999912824849</v>
+        <v>9.96199991282238</v>
       </c>
       <c r="M30" t="n">
-        <v>1.379092427421123e-26</v>
+        <v>2.218214724239183e-26</v>
       </c>
       <c r="N30" t="n">
-        <v>5.188716471430574e-13</v>
+        <v>7.163084764727095e-13</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2020,7 +2020,7 @@
         </is>
       </c>
       <c r="P30" t="n">
-        <v>0.0003188000000022839</v>
+        <v>0.000276299999999452</v>
       </c>
     </row>
     <row r="31">
@@ -2040,13 +2040,13 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>10.00000000000152</v>
+        <v>10.0000000000021</v>
       </c>
       <c r="G31" t="n">
-        <v>155.4767974026128</v>
+        <v>155.476797402612</v>
       </c>
       <c r="H31" t="n">
-        <v>6.418871582732997</v>
+        <v>6.418871582733561</v>
       </c>
       <c r="I31" t="n">
         <v>85.08185965409687</v>
@@ -2055,16 +2055,16 @@
         <v>4.383667298314077</v>
       </c>
       <c r="K31" t="n">
-        <v>85.08185965409763</v>
+        <v>85.08185965409794</v>
       </c>
       <c r="L31" t="n">
-        <v>4.383667298315092</v>
+        <v>4.383667298315471</v>
       </c>
       <c r="M31" t="n">
-        <v>1.291723686148449e-25</v>
+        <v>2.464502488905835e-25</v>
       </c>
       <c r="N31" t="n">
-        <v>1.19717346118935e-12</v>
+        <v>1.666187318928128e-12</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="P31" t="n">
-        <v>0.0002947999999918238</v>
+        <v>0.000237099999999657</v>
       </c>
     </row>
     <row r="32">
@@ -2092,13 +2092,13 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>10.00000000000077</v>
+        <v>9.999999999998343</v>
       </c>
       <c r="G32" t="n">
-        <v>115.9458364923005</v>
+        <v>115.9458364922994</v>
       </c>
       <c r="H32" t="n">
-        <v>7.568981875622266</v>
+        <v>7.568981875619564</v>
       </c>
       <c r="I32" t="n">
         <v>69.94009040741105</v>
@@ -2107,16 +2107,16 @@
         <v>9.94082687493656</v>
       </c>
       <c r="K32" t="n">
-        <v>69.94009040741133</v>
+        <v>69.94009040741032</v>
       </c>
       <c r="L32" t="n">
-        <v>9.940826874937933</v>
+        <v>9.940826874934977</v>
       </c>
       <c r="M32" t="n">
-        <v>2.090124109514682e-26</v>
+        <v>9.054895147886716e-26</v>
       </c>
       <c r="N32" t="n">
-        <v>5.928582565765519e-13</v>
+        <v>1.078628681810331e-12</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2124,7 +2124,7 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>0.000362400000000207</v>
+        <v>0.0005682999999994109</v>
       </c>
     </row>
     <row r="33">
@@ -2144,13 +2144,13 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>9.999999999999394</v>
+        <v>10.00000000000019</v>
       </c>
       <c r="G33" t="n">
-        <v>51.48968789889207</v>
+        <v>51.48968789889289</v>
       </c>
       <c r="H33" t="n">
-        <v>14.49726679822704</v>
+        <v>14.49726679822843</v>
       </c>
       <c r="I33" t="n">
         <v>39.0616009844012</v>
@@ -2159,16 +2159,16 @@
         <v>23.45979414801152</v>
       </c>
       <c r="K33" t="n">
-        <v>39.06160098440098</v>
+        <v>39.06160098440122</v>
       </c>
       <c r="L33" t="n">
-        <v>23.4597941480104</v>
+        <v>23.45979414801259</v>
       </c>
       <c r="M33" t="n">
-        <v>7.526115838227214e-27</v>
+        <v>2.449636787537205e-27</v>
       </c>
       <c r="N33" t="n">
-        <v>3.211577957301792e-13</v>
+        <v>1.598443785373973e-13</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2176,7 +2176,7 @@
         </is>
       </c>
       <c r="P33" t="n">
-        <v>0.0003269000000045708</v>
+        <v>0.0002420999999994677</v>
       </c>
     </row>
     <row r="34">
@@ -2196,13 +2196,13 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>10.00000000000311</v>
+        <v>9.999999999994461</v>
       </c>
       <c r="G34" t="n">
-        <v>154.6000681127443</v>
+        <v>154.6000681127524</v>
       </c>
       <c r="H34" t="n">
-        <v>7.47253385970674</v>
+        <v>7.472533859697343</v>
       </c>
       <c r="I34" t="n">
         <v>98.12939238316436</v>
@@ -2211,16 +2211,16 @@
         <v>5.067646835573846</v>
       </c>
       <c r="K34" t="n">
-        <v>98.12939238316503</v>
+        <v>98.12939238316339</v>
       </c>
       <c r="L34" t="n">
-        <v>5.067646835575898</v>
+        <v>5.067646835569847</v>
       </c>
       <c r="M34" t="n">
-        <v>2.974013177587477e-25</v>
+        <v>9.128481999793173e-25</v>
       </c>
       <c r="N34" t="n">
-        <v>2.047296770843608e-12</v>
+        <v>3.699852011046369e-12</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
         </is>
       </c>
       <c r="P34" t="n">
-        <v>0.0002953999999988355</v>
+        <v>0.0002361000000004054</v>
       </c>
     </row>
     <row r="35">
@@ -2248,13 +2248,13 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>10.00000000000053</v>
+        <v>9.999999999999668</v>
       </c>
       <c r="G35" t="n">
-        <v>44.73182293879218</v>
+        <v>44.73182293879078</v>
       </c>
       <c r="H35" t="n">
-        <v>8.399705052610186</v>
+        <v>8.399705052609201</v>
       </c>
       <c r="I35" t="n">
         <v>29.60621371940404</v>
@@ -2263,16 +2263,16 @@
         <v>16.7283342947574</v>
       </c>
       <c r="K35" t="n">
-        <v>29.60621371940431</v>
+        <v>29.60621371940389</v>
       </c>
       <c r="L35" t="n">
-        <v>16.72833429475836</v>
+        <v>16.72833429475654</v>
       </c>
       <c r="M35" t="n">
-        <v>1.518850214858435e-26</v>
+        <v>4.834370049810946e-27</v>
       </c>
       <c r="N35" t="n">
-        <v>3.704522524022402e-13</v>
+        <v>2.390309058599848e-13</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2280,7 +2280,7 @@
         </is>
       </c>
       <c r="P35" t="n">
-        <v>0.0002941000000049598</v>
+        <v>0.0002277999999993341</v>
       </c>
     </row>
     <row r="36">
@@ -2300,13 +2300,13 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>10.00000000000003</v>
+        <v>10.00000000000011</v>
       </c>
       <c r="G36" t="n">
-        <v>6.941102558653814</v>
+        <v>6.941102558653789</v>
       </c>
       <c r="H36" t="n">
-        <v>12.36120552629626</v>
+        <v>12.36120552629586</v>
       </c>
       <c r="I36" t="n">
         <v>7.633544320503938</v>
@@ -2315,16 +2315,16 @@
         <v>22.30604591386155</v>
       </c>
       <c r="K36" t="n">
-        <v>7.633544320503963</v>
+        <v>7.633544320503938</v>
       </c>
       <c r="L36" t="n">
-        <v>22.30604591386293</v>
+        <v>22.30604591386252</v>
       </c>
       <c r="M36" t="n">
-        <v>2.98933249138775e-28</v>
+        <v>4.963369172637498e-28</v>
       </c>
       <c r="N36" t="n">
-        <v>1.451906699077598e-13</v>
+        <v>1.222020847925292e-13</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2332,7 +2332,7 @@
         </is>
       </c>
       <c r="P36" t="n">
-        <v>0.000327799999993772</v>
+        <v>0.0002283999999992403</v>
       </c>
     </row>
     <row r="37">
@@ -2352,13 +2352,13 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>9.999999999999822</v>
+        <v>10.00000000000039</v>
       </c>
       <c r="G37" t="n">
-        <v>82.44989068033605</v>
+        <v>82.44989068033679</v>
       </c>
       <c r="H37" t="n">
-        <v>6.700195283578762</v>
+        <v>6.700195283579328</v>
       </c>
       <c r="I37" t="n">
         <v>47.28302978168723</v>
@@ -2367,16 +2367,16 @@
         <v>12.44155687331505</v>
       </c>
       <c r="K37" t="n">
-        <v>47.28302978168713</v>
+        <v>47.28302978168741</v>
       </c>
       <c r="L37" t="n">
-        <v>12.44155687331515</v>
+        <v>12.44155687331603</v>
       </c>
       <c r="M37" t="n">
-        <v>1.5413913976989e-27</v>
+        <v>7.271281976067245e-27</v>
       </c>
       <c r="N37" t="n">
-        <v>1.139498196004059e-13</v>
+        <v>3.311223024523282e-13</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -2384,7 +2384,7 @@
         </is>
       </c>
       <c r="P37" t="n">
-        <v>0.0003183000000035463</v>
+        <v>0.0001906999999992109</v>
       </c>
     </row>
     <row r="38">
@@ -2404,13 +2404,13 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>10.00000000000425</v>
+        <v>9.999999999998725</v>
       </c>
       <c r="G38" t="n">
-        <v>131.1312944872311</v>
+        <v>131.1312944872305</v>
       </c>
       <c r="H38" t="n">
-        <v>10.21937054844841</v>
+        <v>10.2193705484408</v>
       </c>
       <c r="I38" t="n">
         <v>93.75460165970797</v>
@@ -2419,16 +2419,16 @@
         <v>10.42956719317792</v>
       </c>
       <c r="K38" t="n">
-        <v>93.75460165970858</v>
+        <v>93.75460165970777</v>
       </c>
       <c r="L38" t="n">
-        <v>10.42956719318328</v>
+        <v>10.42956719317647</v>
       </c>
       <c r="M38" t="n">
-        <v>2.687819040169154e-25</v>
+        <v>2.417035569062766e-26</v>
       </c>
       <c r="N38" t="n">
-        <v>2.455673886024534e-12</v>
+        <v>7.147011909076758e-13</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2436,7 +2436,7 @@
         </is>
       </c>
       <c r="P38" t="n">
-        <v>0.0005382000000082598</v>
+        <v>0.0002338000000001728</v>
       </c>
     </row>
     <row r="39">
@@ -2456,13 +2456,13 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>9.999999999993499</v>
+        <v>10.00000000000359</v>
       </c>
       <c r="G39" t="n">
-        <v>170.0093885143224</v>
+        <v>170.0093885143114</v>
       </c>
       <c r="H39" t="n">
-        <v>8.569178091645298</v>
+        <v>8.569178091657085</v>
       </c>
       <c r="I39" t="n">
         <v>132.8794796020886</v>
@@ -2471,16 +2471,16 @@
         <v>4.031761962137695</v>
       </c>
       <c r="K39" t="n">
-        <v>132.8794796020928</v>
+        <v>132.8794796020864</v>
       </c>
       <c r="L39" t="n">
-        <v>4.031761962134173</v>
+        <v>4.031761962139787</v>
       </c>
       <c r="M39" t="n">
-        <v>2.240899664867643e-24</v>
+        <v>6.937178712285161e-25</v>
       </c>
       <c r="N39" t="n">
-        <v>4.895375789514872e-12</v>
+        <v>2.732686499857415e-12</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -2488,7 +2488,7 @@
         </is>
       </c>
       <c r="P39" t="n">
-        <v>0.0003726000000057184</v>
+        <v>0.0002212000000003655</v>
       </c>
     </row>
     <row r="40">
@@ -2508,13 +2508,13 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>10.00000000000139</v>
+        <v>9.999999999998918</v>
       </c>
       <c r="G40" t="n">
-        <v>69.25916151301526</v>
+        <v>69.25916151301281</v>
       </c>
       <c r="H40" t="n">
-        <v>13.31649415908972</v>
+        <v>13.31649415908564</v>
       </c>
       <c r="I40" t="n">
         <v>51.01422188754402</v>
@@ -2523,16 +2523,16 @@
         <v>20.73148308181667</v>
       </c>
       <c r="K40" t="n">
-        <v>51.01422188754442</v>
+        <v>51.0142218875437</v>
       </c>
       <c r="L40" t="n">
-        <v>20.73148308181977</v>
+        <v>20.73148308181379</v>
       </c>
       <c r="M40" t="n">
-        <v>4.532258951717363e-26</v>
+        <v>2.74307612831343e-26</v>
       </c>
       <c r="N40" t="n">
-        <v>8.13122162522304e-13</v>
+        <v>6.719004439094446e-13</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2540,7 +2540,7 @@
         </is>
       </c>
       <c r="P40" t="n">
-        <v>0.0003198999999938223</v>
+        <v>0.0002100000000009317</v>
       </c>
     </row>
     <row r="41">
@@ -2560,13 +2560,13 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>9.999999999997991</v>
+        <v>10.00000000000054</v>
       </c>
       <c r="G41" t="n">
-        <v>98.44004810616231</v>
+        <v>98.44004810616444</v>
       </c>
       <c r="H41" t="n">
-        <v>12.57478825538807</v>
+        <v>12.57478825539206</v>
       </c>
       <c r="I41" t="n">
         <v>72.19761816275663</v>
@@ -2575,16 +2575,16 @@
         <v>16.90630795593209</v>
       </c>
       <c r="K41" t="n">
-        <v>72.19761816275614</v>
+        <v>72.1976181627568</v>
       </c>
       <c r="L41" t="n">
-        <v>16.90630795592796</v>
+        <v>16.90630795593278</v>
       </c>
       <c r="M41" t="n">
-        <v>6.048995089093151e-26</v>
+        <v>5.025916242108201e-27</v>
       </c>
       <c r="N41" t="n">
-        <v>1.200407726718155e-12</v>
+        <v>2.833614561279026e-13</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="P41" t="n">
-        <v>0.0003202000000044336</v>
+        <v>0.0001889000000012686</v>
       </c>
     </row>
     <row r="42">
@@ -2612,13 +2612,13 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>9.99999999999975</v>
+        <v>9.999999999999917</v>
       </c>
       <c r="G42" t="n">
-        <v>73.38366505445157</v>
+        <v>73.38366505445164</v>
       </c>
       <c r="H42" t="n">
-        <v>3.664392481342106</v>
+        <v>3.664392481342241</v>
       </c>
       <c r="I42" t="n">
         <v>31.92625942098924</v>
@@ -2627,16 +2627,16 @@
         <v>10.18120494273455</v>
       </c>
       <c r="K42" t="n">
-        <v>31.92625942098906</v>
+        <v>31.92625942098919</v>
       </c>
       <c r="L42" t="n">
-        <v>10.181204942735</v>
+        <v>10.18120494273526</v>
       </c>
       <c r="M42" t="n">
-        <v>7.260105642878722e-27</v>
+        <v>1.00001251113924e-27</v>
       </c>
       <c r="N42" t="n">
-        <v>2.648333579559259e-13</v>
+        <v>1.888939395230877e-13</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -2644,7 +2644,7 @@
         </is>
       </c>
       <c r="P42" t="n">
-        <v>0.0003126000000008844</v>
+        <v>0.0002364999999997508</v>
       </c>
     </row>
     <row r="43">
@@ -2664,13 +2664,13 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>9.999999999999883</v>
+        <v>9.999999999999984</v>
       </c>
       <c r="G43" t="n">
-        <v>45.16625227408841</v>
+        <v>45.16625227408937</v>
       </c>
       <c r="H43" t="n">
-        <v>3.553149848071331</v>
+        <v>3.553149848071298</v>
       </c>
       <c r="I43" t="n">
         <v>21.98281729864149</v>
@@ -2679,16 +2679,16 @@
         <v>11.20442922515501</v>
       </c>
       <c r="K43" t="n">
-        <v>21.9828172986414</v>
+        <v>21.98281729864148</v>
       </c>
       <c r="L43" t="n">
-        <v>11.20442922515447</v>
+        <v>11.2044292251545</v>
       </c>
       <c r="M43" t="n">
-        <v>1.000214493064334e-27</v>
+        <v>2.515348240501044e-28</v>
       </c>
       <c r="N43" t="n">
-        <v>1.278022390122046e-13</v>
+        <v>1.086398050823588e-13</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -2696,7 +2696,7 @@
         </is>
       </c>
       <c r="P43" t="n">
-        <v>0.0003006000000027598</v>
+        <v>0.0001996000000001885</v>
       </c>
     </row>
     <row r="44">
@@ -2716,13 +2716,13 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>9.999999999997357</v>
+        <v>10.00000000000236</v>
       </c>
       <c r="G44" t="n">
-        <v>67.41722139252265</v>
+        <v>67.41722139252741</v>
       </c>
       <c r="H44" t="n">
-        <v>14.40857167691441</v>
+        <v>14.40857167692318</v>
       </c>
       <c r="I44" t="n">
         <v>50.70287428680181</v>
@@ -2731,16 +2731,16 @@
         <v>22.14193003827787</v>
       </c>
       <c r="K44" t="n">
-        <v>50.70287428680107</v>
+        <v>50.70287428680244</v>
       </c>
       <c r="L44" t="n">
-        <v>22.14193003827097</v>
+        <v>22.14193003828379</v>
       </c>
       <c r="M44" t="n">
-        <v>1.421117894036398e-25</v>
+        <v>1.258486760862482e-25</v>
       </c>
       <c r="N44" t="n">
-        <v>1.563742855479745e-12</v>
+        <v>1.381907422018116e-12</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -2748,7 +2748,7 @@
         </is>
       </c>
       <c r="P44" t="n">
-        <v>0.001383000000004131</v>
+        <v>0.0001896000000005671</v>
       </c>
     </row>
     <row r="45">
@@ -2768,13 +2768,13 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>10.00000000000009</v>
+        <v>9.999999999999924</v>
       </c>
       <c r="G45" t="n">
-        <v>20.70982195016028</v>
+        <v>20.70982195015999</v>
       </c>
       <c r="H45" t="n">
-        <v>10.30879847135413</v>
+        <v>10.30879847135402</v>
       </c>
       <c r="I45" t="n">
         <v>16.3064939917049</v>
@@ -2783,16 +2783,16 @@
         <v>19.74929820405307</v>
       </c>
       <c r="K45" t="n">
-        <v>16.30649399170495</v>
+        <v>16.30649399170488</v>
       </c>
       <c r="L45" t="n">
-        <v>19.74929820405309</v>
+        <v>19.7492982040528</v>
       </c>
       <c r="M45" t="n">
-        <v>2.655927660366306e-27</v>
+        <v>1.763975479152231e-27</v>
       </c>
       <c r="N45" t="n">
-        <v>1.043187679648891e-13</v>
+        <v>9.399404244191935e-14</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -2800,7 +2800,7 @@
         </is>
       </c>
       <c r="P45" t="n">
-        <v>0.0003195000000033588</v>
+        <v>0.0002067000000014474</v>
       </c>
     </row>
     <row r="46">
@@ -2820,13 +2820,13 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>9.999999999999508</v>
+        <v>9.999999999999901</v>
       </c>
       <c r="G46" t="n">
-        <v>150.2715867598182</v>
+        <v>150.2715867598176</v>
       </c>
       <c r="H46" t="n">
-        <v>4.257553252438085</v>
+        <v>4.257553252438375</v>
       </c>
       <c r="I46" t="n">
         <v>51.49320715697708</v>
@@ -2835,16 +2835,16 @@
         <v>4.733318900759217</v>
       </c>
       <c r="K46" t="n">
-        <v>51.49320715697649</v>
+        <v>51.49320715697702</v>
       </c>
       <c r="L46" t="n">
-        <v>4.733318900758638</v>
+        <v>4.733318900758886</v>
       </c>
       <c r="M46" t="n">
-        <v>3.440331199198786e-26</v>
+        <v>2.464112158835591e-27</v>
       </c>
       <c r="N46" t="n">
-        <v>5.923315920556395e-13</v>
+        <v>1.851335518251467e-13</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -2852,7 +2852,7 @@
         </is>
       </c>
       <c r="P46" t="n">
-        <v>0.0004039999999889687</v>
+        <v>0.0001899999999999125</v>
       </c>
     </row>
     <row r="47">
@@ -2872,13 +2872,13 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>10.0000000000009</v>
+        <v>9.99999999999743</v>
       </c>
       <c r="G47" t="n">
-        <v>178.022072425607</v>
+        <v>178.0220724256108</v>
       </c>
       <c r="H47" t="n">
-        <v>9.594536722137812</v>
+        <v>9.594536722133521</v>
       </c>
       <c r="I47" t="n">
         <v>159.1796698056864</v>
@@ -2887,16 +2887,16 @@
         <v>4.410985878453859</v>
       </c>
       <c r="K47" t="n">
-        <v>159.1796698056854</v>
+        <v>159.1796698056891</v>
       </c>
       <c r="L47" t="n">
-        <v>4.410985878454425</v>
+        <v>4.410985878452546</v>
       </c>
       <c r="M47" t="n">
-        <v>1.576946462619051e-25</v>
+        <v>1.302331979707477e-24</v>
       </c>
       <c r="N47" t="n">
-        <v>7.685859629228694e-13</v>
+        <v>2.070557112004493e-12</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -2904,7 +2904,7 @@
         </is>
       </c>
       <c r="P47" t="n">
-        <v>0.0003234999999932597</v>
+        <v>0.0002402000000003568</v>
       </c>
     </row>
     <row r="48">
@@ -2924,13 +2924,13 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>9.999999999999874</v>
+        <v>10.00000000001477</v>
       </c>
       <c r="G48" t="n">
-        <v>141.0898231450352</v>
+        <v>141.0898231450336</v>
       </c>
       <c r="H48" t="n">
-        <v>10.61800447263258</v>
+        <v>10.61800447265358</v>
       </c>
       <c r="I48" t="n">
         <v>105.4244541290951</v>
@@ -2939,16 +2939,16 @@
         <v>9.516228537064677</v>
       </c>
       <c r="K48" t="n">
-        <v>105.4244541290952</v>
+        <v>105.4244541290955</v>
       </c>
       <c r="L48" t="n">
-        <v>9.516228537064672</v>
+        <v>9.516228537081387</v>
       </c>
       <c r="M48" t="n">
-        <v>4.867758459342239e-28</v>
+        <v>3.259870990906614e-24</v>
       </c>
       <c r="N48" t="n">
-        <v>5.880768080390165e-14</v>
+        <v>7.952165575260967e-12</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -2956,7 +2956,7 @@
         </is>
       </c>
       <c r="P48" t="n">
-        <v>0.0003053999999877988</v>
+        <v>0.000238999999998768</v>
       </c>
     </row>
     <row r="49">
@@ -2976,13 +2976,13 @@
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>10.00000000000007</v>
+        <v>10.00000000000012</v>
       </c>
       <c r="G49" t="n">
-        <v>20.42792494085692</v>
+        <v>20.42792494085698</v>
       </c>
       <c r="H49" t="n">
-        <v>14.69379713323799</v>
+        <v>14.69379713323809</v>
       </c>
       <c r="I49" t="n">
         <v>17.03401812828383</v>
@@ -2991,16 +2991,16 @@
         <v>25.00422823336124</v>
       </c>
       <c r="K49" t="n">
-        <v>17.03401812828386</v>
+        <v>17.03401812828388</v>
       </c>
       <c r="L49" t="n">
-        <v>25.00422823336239</v>
+        <v>25.00422823336255</v>
       </c>
       <c r="M49" t="n">
-        <v>3.261873435647606e-27</v>
+        <v>4.336147967912988e-27</v>
       </c>
       <c r="N49" t="n">
-        <v>1.712406783024895e-13</v>
+        <v>2.061394395839114e-13</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -3008,7 +3008,7 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>0.0002917000000053349</v>
+        <v>0.0001952999999996763</v>
       </c>
     </row>
     <row r="50">
@@ -3028,13 +3028,13 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>9.999999999999901</v>
+        <v>9.99999999999986</v>
       </c>
       <c r="G50" t="n">
-        <v>3.148248767607485</v>
+        <v>3.14824876760751</v>
       </c>
       <c r="H50" t="n">
-        <v>13.69887920616335</v>
+        <v>13.69887920616351</v>
       </c>
       <c r="I50" t="n">
         <v>4.979091423193565</v>
@@ -3043,16 +3043,16 @@
         <v>23.88762442334499</v>
       </c>
       <c r="K50" t="n">
-        <v>4.979091423193577</v>
+        <v>4.97909142319359</v>
       </c>
       <c r="L50" t="n">
-        <v>23.88762442334622</v>
+        <v>23.88762442334638</v>
       </c>
       <c r="M50" t="n">
-        <v>2.83044004364732e-28</v>
+        <v>7.212101272014771e-28</v>
       </c>
       <c r="N50" t="n">
-        <v>1.316462412228851e-13</v>
+        <v>1.801932824584208e-13</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -3060,7 +3060,7 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>0.000309000000001447</v>
+        <v>0.0001935999999993498</v>
       </c>
     </row>
     <row r="51">
@@ -3080,13 +3080,13 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>10.00000000000044</v>
+        <v>10.00000000000059</v>
       </c>
       <c r="G51" t="n">
-        <v>54.17360205406547</v>
+        <v>54.17360205406496</v>
       </c>
       <c r="H51" t="n">
-        <v>5.964741983542178</v>
+        <v>5.964741983542493</v>
       </c>
       <c r="I51" t="n">
         <v>31.07252442683621</v>
@@ -3095,16 +3095,16 @@
         <v>13.5120365339658</v>
       </c>
       <c r="K51" t="n">
-        <v>31.07252442683646</v>
+        <v>31.07252442683651</v>
       </c>
       <c r="L51" t="n">
-        <v>13.51203653396634</v>
+        <v>13.51203653396684</v>
       </c>
       <c r="M51" t="n">
-        <v>1.254792511452518e-26</v>
+        <v>3.629621926665828e-26</v>
       </c>
       <c r="N51" t="n">
-        <v>3.216253636132505e-13</v>
+        <v>5.169878597108695e-13</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>0.000302399999995373</v>
+        <v>0.0001943000000004247</v>
       </c>
     </row>
     <row r="52">
@@ -3132,13 +3132,13 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>10.00000000000072</v>
+        <v>10.0000000000014</v>
       </c>
       <c r="G52" t="n">
-        <v>89.02829619684525</v>
+        <v>89.02829619684552</v>
       </c>
       <c r="H52" t="n">
-        <v>5.736997253392643</v>
+        <v>5.736997253393316</v>
       </c>
       <c r="I52" t="n">
         <v>47.03792036458195</v>
@@ -3147,16 +3147,16 @@
         <v>11.00547523311644</v>
       </c>
       <c r="K52" t="n">
-        <v>47.03792036458241</v>
+        <v>47.03792036458275</v>
       </c>
       <c r="L52" t="n">
-        <v>11.00547523311792</v>
+        <v>11.00547523311896</v>
       </c>
       <c r="M52" t="n">
-        <v>2.673399096886917e-26</v>
+        <v>1.101886134698783e-25</v>
       </c>
       <c r="N52" t="n">
-        <v>6.374428835489976e-13</v>
+        <v>1.180001497497287e-12</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -3164,7 +3164,7 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>0.0002888000000069724</v>
+        <v>0.0002475000000004002</v>
       </c>
     </row>
     <row r="53">
@@ -3184,13 +3184,13 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>10</v>
+        <v>10.00000000000029</v>
       </c>
       <c r="G53" t="n">
-        <v>121.6316547906398</v>
+        <v>121.6316547906395</v>
       </c>
       <c r="H53" t="n">
-        <v>3.536546186435352</v>
+        <v>3.536546186435551</v>
       </c>
       <c r="I53" t="n">
         <v>42.84508415968962</v>
@@ -3199,16 +3199,16 @@
         <v>7.034854823508725</v>
       </c>
       <c r="K53" t="n">
-        <v>42.84508415968966</v>
+        <v>42.84508415968995</v>
       </c>
       <c r="L53" t="n">
-        <v>7.034854823508956</v>
+        <v>7.034854823509235</v>
       </c>
       <c r="M53" t="n">
-        <v>4.004628301525752e-28</v>
+        <v>9.373577179751536e-27</v>
       </c>
       <c r="N53" t="n">
-        <v>7.815796824989726e-14</v>
+        <v>3.481092046841655e-13</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -3216,7 +3216,7 @@
         </is>
       </c>
       <c r="P53" t="n">
-        <v>0.0003251999999918098</v>
+        <v>0.0002525999999996031</v>
       </c>
     </row>
     <row r="54">
@@ -3236,13 +3236,13 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>10.00000000000009</v>
+        <v>9.999999999999961</v>
       </c>
       <c r="G54" t="n">
-        <v>148.1598613277628</v>
+        <v>148.1598613277633</v>
       </c>
       <c r="H54" t="n">
-        <v>3.313415778838473</v>
+        <v>3.313415778838399</v>
       </c>
       <c r="I54" t="n">
         <v>39.20823517402567</v>
@@ -3251,16 +3251,16 @@
         <v>5.169813417634993</v>
       </c>
       <c r="K54" t="n">
-        <v>39.20823517402583</v>
+        <v>39.20823517402565</v>
       </c>
       <c r="L54" t="n">
-        <v>5.16981341763502</v>
+        <v>5.169813417634917</v>
       </c>
       <c r="M54" t="n">
-        <v>2.259235159482147e-27</v>
+        <v>1.324193500914736e-27</v>
       </c>
       <c r="N54" t="n">
-        <v>1.06448432097678e-13</v>
+        <v>5.766498688740617e-14</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -3268,7 +3268,7 @@
         </is>
       </c>
       <c r="P54" t="n">
-        <v>0.0003011000000014974</v>
+        <v>0.0002070999999990164</v>
       </c>
     </row>
     <row r="55">
@@ -3288,13 +3288,13 @@
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>9.99999999999458</v>
+        <v>9.99999999999098</v>
       </c>
       <c r="G55" t="n">
-        <v>152.3992332978265</v>
+        <v>152.3992332978281</v>
       </c>
       <c r="H55" t="n">
-        <v>9.733986483173302</v>
+        <v>9.733986483168582</v>
       </c>
       <c r="I55" t="n">
         <v>114.2699214848488</v>
@@ -3303,16 +3303,16 @@
         <v>7.220398177179498</v>
       </c>
       <c r="K55" t="n">
-        <v>114.2699214848493</v>
+        <v>114.2699214848497</v>
       </c>
       <c r="L55" t="n">
-        <v>7.220398177174794</v>
+        <v>7.220398177171616</v>
       </c>
       <c r="M55" t="n">
-        <v>5.904140879902699e-25</v>
+        <v>1.636537053176951e-24</v>
       </c>
       <c r="N55" t="n">
-        <v>3.099416634047149e-12</v>
+        <v>5.171631543090431e-12</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -3320,7 +3320,7 @@
         </is>
       </c>
       <c r="P55" t="n">
-        <v>0.0002894999999938364</v>
+        <v>0.0001926000000000982</v>
       </c>
     </row>
     <row r="56">
@@ -3340,13 +3340,13 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>10.00000000000059</v>
+        <v>10.0000000000007</v>
       </c>
       <c r="G56" t="n">
-        <v>75.63293408534007</v>
+        <v>75.63293408534021</v>
       </c>
       <c r="H56" t="n">
-        <v>7.35887396358166</v>
+        <v>7.358873963581781</v>
       </c>
       <c r="I56" t="n">
         <v>45.4456541921149</v>
@@ -3355,16 +3355,16 @@
         <v>13.64739445873363</v>
       </c>
       <c r="K56" t="n">
-        <v>45.44565419211518</v>
+        <v>45.44565419211522</v>
       </c>
       <c r="L56" t="n">
-        <v>13.64739445873551</v>
+        <v>13.64739445873571</v>
       </c>
       <c r="M56" t="n">
-        <v>1.630754934091219e-26</v>
+        <v>2.314968705346355e-26</v>
       </c>
       <c r="N56" t="n">
-        <v>5.345928303242075e-13</v>
+        <v>6.106687305654022e-13</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>0.0002886999999986983</v>
+        <v>0.0002380999999989086</v>
       </c>
     </row>
     <row r="57">
@@ -3392,13 +3392,13 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>9.99999999999989</v>
+        <v>9.999999999999719</v>
       </c>
       <c r="G57" t="n">
-        <v>16.75949160093429</v>
+        <v>16.75949160093412</v>
       </c>
       <c r="H57" t="n">
-        <v>14.65987103987744</v>
+        <v>14.6598710398772</v>
       </c>
       <c r="I57" t="n">
         <v>14.44966940927695</v>
@@ -3407,16 +3407,16 @@
         <v>25.01968713371055</v>
       </c>
       <c r="K57" t="n">
-        <v>14.44966940927691</v>
+        <v>14.44966940927685</v>
       </c>
       <c r="L57" t="n">
-        <v>25.01968713371068</v>
+        <v>25.01968713371022</v>
       </c>
       <c r="M57" t="n">
-        <v>2.90584662901566e-28</v>
+        <v>1.524020952140836e-27</v>
       </c>
       <c r="N57" t="n">
-        <v>2.056005243555266e-14</v>
+        <v>1.010926189571383e-13</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -3424,7 +3424,7 @@
         </is>
       </c>
       <c r="P57" t="n">
-        <v>0.0003274000000033084</v>
+        <v>0.000214499999998452</v>
       </c>
     </row>
     <row r="58">
@@ -3444,13 +3444,13 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>10.00000000000439</v>
+        <v>9.999999999998934</v>
       </c>
       <c r="G58" t="n">
-        <v>177.1545330976554</v>
+        <v>177.1545330976658</v>
       </c>
       <c r="H58" t="n">
-        <v>7.000947192180165</v>
+        <v>7.000947192174793</v>
       </c>
       <c r="I58" t="n">
         <v>122.3917356254008</v>
@@ -3459,16 +3459,16 @@
         <v>1.88002910171164</v>
       </c>
       <c r="K58" t="n">
-        <v>122.3917356253954</v>
+        <v>122.3917356254022</v>
       </c>
       <c r="L58" t="n">
-        <v>1.880029101713423</v>
+        <v>1.880029101711374</v>
       </c>
       <c r="M58" t="n">
-        <v>2.015383136733841e-24</v>
+        <v>1.142006865623251e-25</v>
       </c>
       <c r="N58" t="n">
-        <v>4.698710909442305e-12</v>
+        <v>1.015672712029877e-12</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -3476,7 +3476,7 @@
         </is>
       </c>
       <c r="P58" t="n">
-        <v>0.0002996999999993477</v>
+        <v>0.0002004999999982715</v>
       </c>
     </row>
     <row r="59">
@@ -3496,13 +3496,13 @@
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>9.999999999999865</v>
+        <v>9.999999999999982</v>
       </c>
       <c r="G59" t="n">
-        <v>15.72293572239113</v>
+        <v>15.72293572239146</v>
       </c>
       <c r="H59" t="n">
-        <v>5.765725194620618</v>
+        <v>5.765725194620701</v>
       </c>
       <c r="I59" t="n">
         <v>12.23519148406908</v>
@@ -3511,16 +3511,16 @@
         <v>14.37002887945796</v>
       </c>
       <c r="K59" t="n">
-        <v>12.23519148406898</v>
+        <v>12.23519148406906</v>
       </c>
       <c r="L59" t="n">
-        <v>14.37002887945782</v>
+        <v>14.37002887945803</v>
       </c>
       <c r="M59" t="n">
-        <v>1.570611449529131e-27</v>
+        <v>9.587408711117467e-29</v>
       </c>
       <c r="N59" t="n">
-        <v>1.04742546836513e-13</v>
+        <v>3.23780178877126e-14</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -3528,7 +3528,7 @@
         </is>
       </c>
       <c r="P59" t="n">
-        <v>0.0002960000000058471</v>
+        <v>0.0002030000000008414</v>
       </c>
     </row>
     <row r="60">
@@ -3548,13 +3548,13 @@
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>10.00000000000052</v>
+        <v>10.00000000000104</v>
       </c>
       <c r="G60" t="n">
-        <v>65.71900494408581</v>
+        <v>65.71900494408682</v>
       </c>
       <c r="H60" t="n">
-        <v>8.414470990720611</v>
+        <v>8.41447099072113</v>
       </c>
       <c r="I60" t="n">
         <v>41.96631688030001</v>
@@ -3563,16 +3563,16 @@
         <v>15.51473424919647</v>
       </c>
       <c r="K60" t="n">
-        <v>41.96631688030025</v>
+        <v>41.9663168803005</v>
       </c>
       <c r="L60" t="n">
-        <v>15.5147342491969</v>
+        <v>15.51473424919778</v>
       </c>
       <c r="M60" t="n">
-        <v>9.998778565225107e-27</v>
+        <v>3.811977941371317e-26</v>
       </c>
       <c r="N60" t="n">
-        <v>2.911427089036294e-13</v>
+        <v>6.365339592962822e-13</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -3580,7 +3580,7 @@
         </is>
       </c>
       <c r="P60" t="n">
-        <v>0.0003144000000077085</v>
+        <v>0.0005597000000001628</v>
       </c>
     </row>
     <row r="61">
@@ -3600,13 +3600,13 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>10.00000000000027</v>
+        <v>10.00000000000024</v>
       </c>
       <c r="G61" t="n">
-        <v>166.3263208033956</v>
+        <v>166.3263208033959</v>
       </c>
       <c r="H61" t="n">
-        <v>4.894446966417693</v>
+        <v>4.894446966417688</v>
       </c>
       <c r="I61" t="n">
         <v>56.76408976169788</v>
@@ -3615,16 +3615,16 @@
         <v>3.059300117780022</v>
       </c>
       <c r="K61" t="n">
-        <v>56.76408976169829</v>
+        <v>56.7640897616984</v>
       </c>
       <c r="L61" t="n">
-        <v>3.059300117780028</v>
+        <v>3.059300117779991</v>
       </c>
       <c r="M61" t="n">
-        <v>1.421340074154002e-26</v>
+        <v>1.715499817129727e-26</v>
       </c>
       <c r="N61" t="n">
-        <v>2.224732998533417e-13</v>
+        <v>2.557950385347732e-13</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="P61" t="n">
-        <v>0.0003010000000074342</v>
+        <v>0.0002442000000009159</v>
       </c>
     </row>
     <row r="62">
@@ -3652,13 +3652,13 @@
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>9.999999999999792</v>
+        <v>9.999999999999751</v>
       </c>
       <c r="G62" t="n">
-        <v>54.15719940839111</v>
+        <v>54.15719940839121</v>
       </c>
       <c r="H62" t="n">
-        <v>5.243349796102332</v>
+        <v>5.243349796102261</v>
       </c>
       <c r="I62" t="n">
         <v>29.53509225686502</v>
@@ -3667,16 +3667,16 @@
         <v>12.72106643331113</v>
       </c>
       <c r="K62" t="n">
-        <v>29.53509225686491</v>
+        <v>29.53509225686488</v>
       </c>
       <c r="L62" t="n">
-        <v>12.72106643331103</v>
+        <v>12.72106643331091</v>
       </c>
       <c r="M62" t="n">
-        <v>3.832270392112404e-27</v>
+        <v>6.564412565547425e-27</v>
       </c>
       <c r="N62" t="n">
-        <v>1.459601702308243e-13</v>
+        <v>1.992292658238577e-13</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -3684,7 +3684,7 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>0.0002963999999963107</v>
+        <v>0.0002027999999985042</v>
       </c>
     </row>
     <row r="63">
@@ -3704,13 +3704,13 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>9.999999999999204</v>
+        <v>10.00000000000088</v>
       </c>
       <c r="G63" t="n">
-        <v>148.4045056643923</v>
+        <v>148.4045056643894</v>
       </c>
       <c r="H63" t="n">
-        <v>5.176196789965732</v>
+        <v>5.176196789967141</v>
       </c>
       <c r="I63" t="n">
         <v>64.68552660313826</v>
@@ -3719,16 +3719,16 @@
         <v>4.894765047516295</v>
       </c>
       <c r="K63" t="n">
-        <v>64.68552660313762</v>
+        <v>64.68552660313914</v>
       </c>
       <c r="L63" t="n">
-        <v>4.894765047515858</v>
+        <v>4.894765047517073</v>
       </c>
       <c r="M63" t="n">
-        <v>5.803640911950914e-26</v>
+        <v>7.793617333455979e-26</v>
       </c>
       <c r="N63" t="n">
-        <v>6.654925544087476e-13</v>
+        <v>8.776376850202122e-13</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -3736,7 +3736,7 @@
         </is>
       </c>
       <c r="P63" t="n">
-        <v>0.0003305000000040081</v>
+        <v>0.0001929999999994436</v>
       </c>
     </row>
     <row r="64">
@@ -3756,13 +3756,13 @@
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>9.999999999999924</v>
+        <v>10.00000000000001</v>
       </c>
       <c r="G64" t="n">
-        <v>6.075847876177366</v>
+        <v>6.07584787617743</v>
       </c>
       <c r="H64" t="n">
-        <v>8.869290095586969</v>
+        <v>8.869290095586843</v>
       </c>
       <c r="I64" t="n">
         <v>7.285415246674767</v>
@@ -3774,13 +3774,13 @@
         <v>7.285415246674729</v>
       </c>
       <c r="L64" t="n">
-        <v>18.11323190547843</v>
+        <v>18.11323190547837</v>
       </c>
       <c r="M64" t="n">
-        <v>2.472258763147707e-28</v>
+        <v>3.961538824172415e-28</v>
       </c>
       <c r="N64" t="n">
-        <v>6.355807861213682e-14</v>
+        <v>1.025337345400049e-13</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -3788,7 +3788,7 @@
         </is>
       </c>
       <c r="P64" t="n">
-        <v>0.000304799999994998</v>
+        <v>0.0001978000000004698</v>
       </c>
     </row>
     <row r="65">
@@ -3808,13 +3808,13 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>10.00000000000077</v>
+        <v>9.999999999999636</v>
       </c>
       <c r="G65" t="n">
-        <v>99.70938405010622</v>
+        <v>99.70938405010504</v>
       </c>
       <c r="H65" t="n">
-        <v>7.754974724465271</v>
+        <v>7.754974724464016</v>
       </c>
       <c r="I65" t="n">
         <v>60.6583617383578</v>
@@ -3823,16 +3823,16 @@
         <v>11.86528034063046</v>
       </c>
       <c r="K65" t="n">
-        <v>60.65836173835814</v>
+        <v>60.65836173835763</v>
       </c>
       <c r="L65" t="n">
-        <v>11.86528034063195</v>
+        <v>11.86528034063034</v>
       </c>
       <c r="M65" t="n">
-        <v>2.147707473176206e-26</v>
+        <v>4.538601184165307e-27</v>
       </c>
       <c r="N65" t="n">
-        <v>5.912641093610988e-13</v>
+        <v>1.971169613156882e-13</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -3840,7 +3840,7 @@
         </is>
       </c>
       <c r="P65" t="n">
-        <v>0.0002903000000031852</v>
+        <v>0.0003119999999992018</v>
       </c>
     </row>
     <row r="66">
@@ -3860,13 +3860,13 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>9.999999999999662</v>
+        <v>10.00000000000016</v>
       </c>
       <c r="G66" t="n">
-        <v>68.23773457807778</v>
+        <v>68.23773457807839</v>
       </c>
       <c r="H66" t="n">
-        <v>9.805178006155073</v>
+        <v>9.805178006155719</v>
       </c>
       <c r="I66" t="n">
         <v>45.8459076388655</v>
@@ -3875,16 +3875,16 @@
         <v>16.86218162216168</v>
       </c>
       <c r="K66" t="n">
-        <v>45.84590763886533</v>
+        <v>45.84590763886551</v>
       </c>
       <c r="L66" t="n">
-        <v>16.86218162216194</v>
+        <v>16.86218162216296</v>
       </c>
       <c r="M66" t="n">
-        <v>4.574890603373821e-27</v>
+        <v>7.029442284421642e-27</v>
       </c>
       <c r="N66" t="n">
-        <v>1.655705598228495e-13</v>
+        <v>2.216740792941347e-13</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="P66" t="n">
-        <v>0.000885100000004968</v>
+        <v>0.0001923000000001451</v>
       </c>
     </row>
     <row r="67">
@@ -3912,13 +3912,13 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>9.999999999999714</v>
+        <v>9.999999999999877</v>
       </c>
       <c r="G67" t="n">
-        <v>39.35610902649593</v>
+        <v>39.35610902649603</v>
       </c>
       <c r="H67" t="n">
-        <v>3.376832634030802</v>
+        <v>3.376832634031</v>
       </c>
       <c r="I67" t="n">
         <v>19.57687427078943</v>
@@ -3927,16 +3927,16 @@
         <v>11.16212898988536</v>
       </c>
       <c r="K67" t="n">
-        <v>19.57687427078918</v>
+        <v>19.57687427078934</v>
       </c>
       <c r="L67" t="n">
-        <v>11.1621289898853</v>
+        <v>11.16212898988567</v>
       </c>
       <c r="M67" t="n">
-        <v>7.955125447126374e-27</v>
+        <v>1.196002305788558e-27</v>
       </c>
       <c r="N67" t="n">
-        <v>2.237463952715837e-13</v>
+        <v>1.188825332662821e-13</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -3944,7 +3944,7 @@
         </is>
       </c>
       <c r="P67" t="n">
-        <v>0.000325399999994147</v>
+        <v>0.0001887000000007077</v>
       </c>
     </row>
     <row r="68">
@@ -3964,13 +3964,13 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>10.00000000000006</v>
+        <v>9.999999999999776</v>
       </c>
       <c r="G68" t="n">
-        <v>27.77176406363001</v>
+        <v>27.77176406362915</v>
       </c>
       <c r="H68" t="n">
-        <v>4.604394728400742</v>
+        <v>4.604394728400519</v>
       </c>
       <c r="I68" t="n">
         <v>16.96964631110587</v>
@@ -3979,16 +3979,16 @@
         <v>12.83113260813786</v>
       </c>
       <c r="K68" t="n">
-        <v>16.9696463111059</v>
+        <v>16.96964631110568</v>
       </c>
       <c r="L68" t="n">
-        <v>12.83113260813693</v>
+        <v>12.83113260813641</v>
       </c>
       <c r="M68" t="n">
-        <v>3.078204538429007e-28</v>
+        <v>7.213178508948605e-27</v>
       </c>
       <c r="N68" t="n">
-        <v>1.649456820283341e-13</v>
+        <v>3.981463869494745e-13</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -3996,7 +3996,7 @@
         </is>
       </c>
       <c r="P68" t="n">
-        <v>0.0002965000000045848</v>
+        <v>0.0001873999999997267</v>
       </c>
     </row>
     <row r="69">
@@ -4016,13 +4016,13 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>10.00000000000259</v>
+        <v>10.00000000000391</v>
       </c>
       <c r="G69" t="n">
-        <v>98.25325738829797</v>
+        <v>98.25325738829919</v>
       </c>
       <c r="H69" t="n">
-        <v>13.30627932710062</v>
+        <v>13.30627932710275</v>
       </c>
       <c r="I69" t="n">
         <v>73.30159050095429</v>
@@ -4031,16 +4031,16 @@
         <v>17.71985515776622</v>
       </c>
       <c r="K69" t="n">
-        <v>73.30159050095484</v>
+        <v>73.3015905009552</v>
       </c>
       <c r="L69" t="n">
-        <v>17.7198551577716</v>
+        <v>17.71985515777416</v>
       </c>
       <c r="M69" t="n">
-        <v>9.413542669996755e-26</v>
+        <v>1.981763836430752e-25</v>
       </c>
       <c r="N69" t="n">
-        <v>1.504493467336992e-12</v>
+        <v>2.260729411974127e-12</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -4048,7 +4048,7 @@
         </is>
       </c>
       <c r="P69" t="n">
-        <v>0.000293400000003885</v>
+        <v>0.0001886999999989314</v>
       </c>
     </row>
     <row r="70">
@@ -4068,13 +4068,13 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>9.999999999999988</v>
+        <v>9.999999999999744</v>
       </c>
       <c r="G70" t="n">
-        <v>46.68686459072021</v>
+        <v>46.68686459071845</v>
       </c>
       <c r="H70" t="n">
-        <v>3.520332613942736</v>
+        <v>3.520332613942712</v>
       </c>
       <c r="I70" t="n">
         <v>22.43075918953557</v>
@@ -4083,16 +4083,16 @@
         <v>11.12306944814092</v>
       </c>
       <c r="K70" t="n">
-        <v>22.43075918953555</v>
+        <v>22.43075918953536</v>
       </c>
       <c r="L70" t="n">
-        <v>11.12306944814057</v>
+        <v>11.12306944814037</v>
       </c>
       <c r="M70" t="n">
-        <v>5.081865235359174e-28</v>
+        <v>4.999995228387835e-27</v>
       </c>
       <c r="N70" t="n">
-        <v>1.097870947935543e-13</v>
+        <v>2.299429301570162e-13</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -4100,7 +4100,7 @@
         </is>
       </c>
       <c r="P70" t="n">
-        <v>0.0003176000000024715</v>
+        <v>0.0002583999999998809</v>
       </c>
     </row>
     <row r="71">
@@ -4120,31 +4120,31 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>10.00000000000088</v>
+        <v>10.00000000000037</v>
       </c>
       <c r="G71" t="n">
-        <v>53.32484910103915</v>
+        <v>53.3248491010383</v>
       </c>
       <c r="H71" t="n">
-        <v>12.70881258808121</v>
+        <v>12.7088125880806</v>
       </c>
       <c r="I71" t="n">
-        <v>39.09766949772916</v>
+        <v>39.09766949772915</v>
       </c>
       <c r="J71" t="n">
         <v>21.2511977384674</v>
       </c>
       <c r="K71" t="n">
-        <v>39.09766949772946</v>
+        <v>39.09766949772926</v>
       </c>
       <c r="L71" t="n">
-        <v>21.25119773847</v>
+        <v>21.25119773846895</v>
       </c>
       <c r="M71" t="n">
-        <v>1.95694227765598e-26</v>
+        <v>7.046880057288068e-27</v>
       </c>
       <c r="N71" t="n">
-        <v>5.639363075478391e-13</v>
+        <v>2.911918477670848e-13</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -4152,7 +4152,7 @@
         </is>
       </c>
       <c r="P71" t="n">
-        <v>0.0002863999999931366</v>
+        <v>0.0005140000000007916</v>
       </c>
     </row>
     <row r="72">
@@ -4172,13 +4172,13 @@
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>10.00000000000001</v>
+        <v>10.00000000000313</v>
       </c>
       <c r="G72" t="n">
-        <v>166.9464969514125</v>
+        <v>166.9464969514109</v>
       </c>
       <c r="H72" t="n">
-        <v>13.4691155329106</v>
+        <v>13.46911553291563</v>
       </c>
       <c r="I72" t="n">
         <v>150.0337683635548</v>
@@ -4187,16 +4187,16 @@
         <v>9.651912212970135</v>
       </c>
       <c r="K72" t="n">
-        <v>150.0337683635548</v>
+        <v>150.0337683635534</v>
       </c>
       <c r="L72" t="n">
-        <v>9.651912212970187</v>
+        <v>9.651912212973375</v>
       </c>
       <c r="M72" t="n">
-        <v>2.206248144449652e-28</v>
+        <v>1.444849460575151e-24</v>
       </c>
       <c r="N72" t="n">
-        <v>1.290299671322505e-14</v>
+        <v>1.890645028681704e-12</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -4204,7 +4204,7 @@
         </is>
       </c>
       <c r="P72" t="n">
-        <v>0.0002867000000037478</v>
+        <v>0.0002297000000002214</v>
       </c>
     </row>
     <row r="73">
@@ -4224,13 +4224,13 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>10.00000000000009</v>
+        <v>9.999999999999908</v>
       </c>
       <c r="G73" t="n">
-        <v>33.40354946733702</v>
+        <v>33.40354946733678</v>
       </c>
       <c r="H73" t="n">
-        <v>7.639191636505086</v>
+        <v>7.63919163650483</v>
       </c>
       <c r="I73" t="n">
         <v>22.46395608561936</v>
@@ -4239,16 +4239,16 @@
         <v>16.27104575612665</v>
       </c>
       <c r="K73" t="n">
-        <v>22.46395608561941</v>
+        <v>22.46395608561931</v>
       </c>
       <c r="L73" t="n">
-        <v>16.27104575612675</v>
+        <v>16.27104575612629</v>
       </c>
       <c r="M73" t="n">
-        <v>2.537431597644629e-27</v>
+        <v>4.053103963548256e-28</v>
       </c>
       <c r="N73" t="n">
-        <v>1.063356284385313e-13</v>
+        <v>6.19230401147662e-14</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -4256,7 +4256,7 @@
         </is>
       </c>
       <c r="P73" t="n">
-        <v>0.0003238999999979342</v>
+        <v>0.0001886999999989314</v>
       </c>
     </row>
     <row r="74">
@@ -4276,13 +4276,13 @@
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>10.00000000000017</v>
+        <v>9.999999999999899</v>
       </c>
       <c r="G74" t="n">
-        <v>19.21287640595617</v>
+        <v>19.21287640595582</v>
       </c>
       <c r="H74" t="n">
-        <v>11.21211159934452</v>
+        <v>11.21211159934397</v>
       </c>
       <c r="I74" t="n">
         <v>15.57133329969279</v>
@@ -4291,16 +4291,16 @@
         <v>20.85419847183129</v>
       </c>
       <c r="K74" t="n">
-        <v>15.57133329969287</v>
+        <v>15.57133329969274</v>
       </c>
       <c r="L74" t="n">
-        <v>20.85419847183192</v>
+        <v>20.854198471831</v>
       </c>
       <c r="M74" t="n">
-        <v>1.544488453883671e-27</v>
+        <v>1.37590087373874e-27</v>
       </c>
       <c r="N74" t="n">
-        <v>1.384248077745576e-13</v>
+        <v>1.01668256283347e-13</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -4308,7 +4308,7 @@
         </is>
       </c>
       <c r="P74" t="n">
-        <v>0.0002969999999891115</v>
+        <v>0.0002470999999992785</v>
       </c>
     </row>
     <row r="75">
@@ -4328,13 +4328,13 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>9.999999999995467</v>
+        <v>9.999999999999305</v>
       </c>
       <c r="G75" t="n">
-        <v>115.684184841492</v>
+        <v>115.6841848414939</v>
       </c>
       <c r="H75" t="n">
-        <v>9.463451171621461</v>
+        <v>9.463451171626449</v>
       </c>
       <c r="I75" t="n">
         <v>77.81913838663891</v>
@@ -4343,16 +4343,16 @@
         <v>11.66724248977646</v>
       </c>
       <c r="K75" t="n">
-        <v>77.81913838663762</v>
+        <v>77.81913838663874</v>
       </c>
       <c r="L75" t="n">
-        <v>11.66724248977031</v>
+        <v>11.66724248977561</v>
       </c>
       <c r="M75" t="n">
-        <v>4.301283909902121e-25</v>
+        <v>1.103444930205694e-26</v>
       </c>
       <c r="N75" t="n">
-        <v>2.819417565863713e-12</v>
+        <v>4.122354055291835e-13</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -4360,7 +4360,7 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>0.0002881999999999607</v>
+        <v>0.0001895999999987907</v>
       </c>
     </row>
     <row r="76">
@@ -4380,13 +4380,13 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>10.0000000000003</v>
+        <v>10.00000000000051</v>
       </c>
       <c r="G76" t="n">
-        <v>36.39641281744385</v>
+        <v>36.39641281744418</v>
       </c>
       <c r="H76" t="n">
-        <v>12.41457124932714</v>
+        <v>12.41457124932738</v>
       </c>
       <c r="I76" t="n">
         <v>27.32317301036183</v>
@@ -4395,16 +4395,16 @@
         <v>21.80818795837916</v>
       </c>
       <c r="K76" t="n">
-        <v>27.32317301036195</v>
+        <v>27.32317301036203</v>
       </c>
       <c r="L76" t="n">
-        <v>21.80818795838057</v>
+        <v>21.80818795838102</v>
       </c>
       <c r="M76" t="n">
-        <v>2.679896182144099e-27</v>
+        <v>6.954910954062041e-27</v>
       </c>
       <c r="N76" t="n">
-        <v>2.295075108927319e-13</v>
+        <v>3.400639390776264e-13</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -4412,7 +4412,7 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>0.0003832999999957565</v>
+        <v>0.0002069000000002319</v>
       </c>
     </row>
     <row r="77">
@@ -4432,13 +4432,13 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>9.999999999999819</v>
+        <v>10.00000000000063</v>
       </c>
       <c r="G77" t="n">
-        <v>102.409239621464</v>
+        <v>102.4092396214662</v>
       </c>
       <c r="H77" t="n">
-        <v>3.79157073107318</v>
+        <v>3.791570731073712</v>
       </c>
       <c r="I77" t="n">
         <v>41.23088095385175</v>
@@ -4447,16 +4447,16 @@
         <v>8.517806771190989</v>
       </c>
       <c r="K77" t="n">
-        <v>41.23088095385158</v>
+        <v>41.23088095385234</v>
       </c>
       <c r="L77" t="n">
-        <v>8.517806771190473</v>
+        <v>8.517806771191234</v>
       </c>
       <c r="M77" t="n">
-        <v>2.865382916688542e-27</v>
+        <v>3.530724843409083e-26</v>
       </c>
       <c r="N77" t="n">
-        <v>2.347407226144867e-13</v>
+        <v>5.127922491916518e-13</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -4464,7 +4464,7 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>0.0003161000000062586</v>
+        <v>0.0001933000000011731</v>
       </c>
     </row>
     <row r="78">
@@ -4484,13 +4484,13 @@
         <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>10.00000000000085</v>
+        <v>10.00000000000193</v>
       </c>
       <c r="G78" t="n">
-        <v>55.94936395614484</v>
+        <v>55.94936395614604</v>
       </c>
       <c r="H78" t="n">
-        <v>12.82784664862759</v>
+        <v>12.82784664862931</v>
       </c>
       <c r="I78" t="n">
         <v>41.02759868558736</v>
@@ -4499,16 +4499,16 @@
         <v>21.21280471567252</v>
       </c>
       <c r="K78" t="n">
-        <v>41.02759868558763</v>
+        <v>41.02759868558799</v>
       </c>
       <c r="L78" t="n">
-        <v>21.212804715675</v>
+        <v>21.21280471567772</v>
       </c>
       <c r="M78" t="n">
-        <v>2.29478397829865e-26</v>
+        <v>1.113436807721812e-25</v>
       </c>
       <c r="N78" t="n">
-        <v>5.603866976263716e-13</v>
+        <v>1.222759861800907e-12</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -4516,7 +4516,7 @@
         </is>
       </c>
       <c r="P78" t="n">
-        <v>0.0003229000000004589</v>
+        <v>0.0001942000000010324</v>
       </c>
     </row>
     <row r="79">
@@ -4536,13 +4536,13 @@
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>9.999999999998709</v>
+        <v>9.999999999991706</v>
       </c>
       <c r="G79" t="n">
-        <v>165.4396257238535</v>
+        <v>165.4396257238582</v>
       </c>
       <c r="H79" t="n">
-        <v>10.70634719908449</v>
+        <v>10.70634719907489</v>
       </c>
       <c r="I79" t="n">
         <v>138.9401716507728</v>
@@ -4551,16 +4551,16 @@
         <v>6.69919649565565</v>
       </c>
       <c r="K79" t="n">
-        <v>138.9401716507734</v>
+        <v>138.9401716507766</v>
       </c>
       <c r="L79" t="n">
-        <v>6.699196495654619</v>
+        <v>6.699196495649128</v>
       </c>
       <c r="M79" t="n">
-        <v>1.148983411207283e-25</v>
+        <v>4.646228459649902e-24</v>
       </c>
       <c r="N79" t="n">
-        <v>8.328025034658153e-13</v>
+        <v>5.381028977718728e-12</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -4568,7 +4568,7 @@
         </is>
       </c>
       <c r="P79" t="n">
-        <v>0.0006089000000031319</v>
+        <v>0.0002341999999995181</v>
       </c>
     </row>
     <row r="80">
@@ -4588,13 +4588,13 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>9.999999999999886</v>
+        <v>10.0000000000001</v>
       </c>
       <c r="G80" t="n">
-        <v>8.672620950042585</v>
+        <v>8.672620950042903</v>
       </c>
       <c r="H80" t="n">
-        <v>11.17155616641232</v>
+        <v>11.17155616641261</v>
       </c>
       <c r="I80" t="n">
         <v>8.792537788842502</v>
@@ -4603,16 +4603,16 @@
         <v>20.88161751407274</v>
       </c>
       <c r="K80" t="n">
-        <v>8.792537788842425</v>
+        <v>8.792537788842527</v>
       </c>
       <c r="L80" t="n">
-        <v>20.88161751407308</v>
+        <v>20.88161751407366</v>
       </c>
       <c r="M80" t="n">
-        <v>1.413334857189451e-27</v>
+        <v>2.35376270042603e-28</v>
       </c>
       <c r="N80" t="n">
-        <v>1.20011257552149e-13</v>
+        <v>8.361752925562535e-14</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -4620,7 +4620,7 @@
         </is>
       </c>
       <c r="P80" t="n">
-        <v>0.0003230999999885853</v>
+        <v>0.0001902999999998656</v>
       </c>
     </row>
     <row r="81">
@@ -4640,13 +4640,13 @@
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>10.00000000000044</v>
+        <v>10.00000000000103</v>
       </c>
       <c r="G81" t="n">
-        <v>90.12026274126919</v>
+        <v>90.1202627412698</v>
       </c>
       <c r="H81" t="n">
-        <v>8.616809111377888</v>
+        <v>8.616809111378599</v>
       </c>
       <c r="I81" t="n">
         <v>57.39789300421757</v>
@@ -4655,16 +4655,16 @@
         <v>13.66352932901044</v>
       </c>
       <c r="K81" t="n">
-        <v>57.39789300421778</v>
+        <v>57.39789300421801</v>
       </c>
       <c r="L81" t="n">
-        <v>13.6635293290111</v>
+        <v>13.66352932901208</v>
       </c>
       <c r="M81" t="n">
-        <v>5.796275304415828e-27</v>
+        <v>3.328810245623681e-26</v>
       </c>
       <c r="N81" t="n">
-        <v>2.905685905028589e-13</v>
+        <v>6.888007403834788e-13</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -4672,7 +4672,7 @@
         </is>
       </c>
       <c r="P81" t="n">
-        <v>0.000296700000006922</v>
+        <v>0.0001853999999994471</v>
       </c>
     </row>
     <row r="82">
@@ -4692,13 +4692,13 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>10.00000000000206</v>
+        <v>10.00000000000218</v>
       </c>
       <c r="G82" t="n">
-        <v>93.94482897004751</v>
+        <v>93.94482897004808</v>
       </c>
       <c r="H82" t="n">
-        <v>11.39287640417902</v>
+        <v>11.3928764041791</v>
       </c>
       <c r="I82" t="n">
         <v>66.48783954982605</v>
@@ -4707,16 +4707,16 @@
         <v>16.15039452812126</v>
       </c>
       <c r="K82" t="n">
-        <v>66.4878395498266</v>
+        <v>66.48783954982675</v>
       </c>
       <c r="L82" t="n">
-        <v>16.15039452812498</v>
+        <v>16.15039452812505</v>
       </c>
       <c r="M82" t="n">
-        <v>8.811565839543548e-26</v>
+        <v>8.502055470260694e-26</v>
       </c>
       <c r="N82" t="n">
-        <v>1.236894737080728e-12</v>
+        <v>1.302841480488922e-12</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -4724,7 +4724,7 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>0.000293299999995611</v>
+        <v>0.0002258000000008309</v>
       </c>
     </row>
     <row r="83">
@@ -4744,13 +4744,13 @@
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>9.999999999999577</v>
+        <v>9.999999999999346</v>
       </c>
       <c r="G83" t="n">
-        <v>63.97544120494177</v>
+        <v>63.97544120494143</v>
       </c>
       <c r="H83" t="n">
-        <v>7.090186520271216</v>
+        <v>7.090186520270968</v>
       </c>
       <c r="I83" t="n">
         <v>38.4159118793041</v>
@@ -4759,16 +4759,16 @@
         <v>14.1881020213233</v>
       </c>
       <c r="K83" t="n">
-        <v>38.41591187930388</v>
+        <v>38.41591187930376</v>
       </c>
       <c r="L83" t="n">
-        <v>14.18810202132245</v>
+        <v>14.18810202132202</v>
       </c>
       <c r="M83" t="n">
-        <v>8.254664642040431e-27</v>
+        <v>2.086291502486028e-26</v>
       </c>
       <c r="N83" t="n">
-        <v>3.19078950013323e-13</v>
+        <v>4.937954417667624e-13</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -4776,7 +4776,7 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>0.0003218000000089205</v>
+        <v>0.0002921000000011276</v>
       </c>
     </row>
     <row r="84">
@@ -4796,13 +4796,13 @@
         <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>10.00000000000029</v>
+        <v>9.999999999999627</v>
       </c>
       <c r="G84" t="n">
-        <v>49.54062056424092</v>
+        <v>49.54062056424031</v>
       </c>
       <c r="H84" t="n">
-        <v>10.67076913110379</v>
+        <v>10.6707691311027</v>
       </c>
       <c r="I84" t="n">
         <v>34.81590641774923</v>
@@ -4811,16 +4811,16 @@
         <v>19.11454519061216</v>
       </c>
       <c r="K84" t="n">
-        <v>34.81590641774933</v>
+        <v>34.8159064177491</v>
       </c>
       <c r="L84" t="n">
-        <v>19.11454519061329</v>
+        <v>19.11454519061152</v>
       </c>
       <c r="M84" t="n">
-        <v>7.795223089760476e-27</v>
+        <v>5.704373528498164e-27</v>
       </c>
       <c r="N84" t="n">
-        <v>2.598061419530847e-13</v>
+        <v>2.26781267608343e-13</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -4828,7 +4828,7 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>0.0002949000000000979</v>
+        <v>0.0002405999999997022</v>
       </c>
     </row>
     <row r="85">
@@ -4848,13 +4848,13 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>10.0000000000006</v>
+        <v>10.00000000000002</v>
       </c>
       <c r="G85" t="n">
-        <v>46.26763687892571</v>
+        <v>46.26763687892535</v>
       </c>
       <c r="H85" t="n">
-        <v>11.20545099685391</v>
+        <v>11.20545099685281</v>
       </c>
       <c r="I85" t="n">
         <v>33.13287081288786</v>
@@ -4863,16 +4863,16 @@
         <v>19.91760304290331</v>
       </c>
       <c r="K85" t="n">
-        <v>33.13287081288809</v>
+        <v>33.13287081288789</v>
       </c>
       <c r="L85" t="n">
-        <v>19.91760304290522</v>
+        <v>19.91760304290347</v>
       </c>
       <c r="M85" t="n">
-        <v>2.240726882412722e-26</v>
+        <v>4.995686280652502e-28</v>
       </c>
       <c r="N85" t="n">
-        <v>4.626055274272034e-13</v>
+        <v>3.713128110498342e-14</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -4880,7 +4880,7 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>0.0002957000000094467</v>
+        <v>0.0002028999999996728</v>
       </c>
     </row>
     <row r="86">
@@ -4900,13 +4900,13 @@
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>9.999999999999897</v>
+        <v>10.00000000000001</v>
       </c>
       <c r="G86" t="n">
-        <v>8.287378853667258</v>
+        <v>8.287378853667359</v>
       </c>
       <c r="H86" t="n">
-        <v>7.442907793387278</v>
+        <v>7.442907793387066</v>
       </c>
       <c r="I86" t="n">
         <v>8.615529210004841</v>
@@ -4915,16 +4915,16 @@
         <v>16.40699998673912</v>
       </c>
       <c r="K86" t="n">
-        <v>8.615529210004816</v>
+        <v>8.615529210004828</v>
       </c>
       <c r="L86" t="n">
-        <v>16.40699998673909</v>
+        <v>16.40699998673894</v>
       </c>
       <c r="M86" t="n">
-        <v>3.207472970489018e-28</v>
+        <v>2.95162919870358e-28</v>
       </c>
       <c r="N86" t="n">
-        <v>4.2781678158363e-14</v>
+        <v>6.016061688587403e-14</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>0.0005560999999971727</v>
+        <v>0.0001888000000001</v>
       </c>
     </row>
     <row r="87">
@@ -4952,13 +4952,13 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>9.99999999999735</v>
+        <v>9.999999999998403</v>
       </c>
       <c r="G87" t="n">
-        <v>111.6672866195844</v>
+        <v>111.667286619585</v>
       </c>
       <c r="H87" t="n">
-        <v>9.107436823741546</v>
+        <v>9.107436823742884</v>
       </c>
       <c r="I87" t="n">
         <v>73.53144854422638</v>
@@ -4967,16 +4967,16 @@
         <v>11.81175051977503</v>
       </c>
       <c r="K87" t="n">
-        <v>73.53144854422553</v>
+        <v>73.53144854422582</v>
       </c>
       <c r="L87" t="n">
-        <v>11.81175051977134</v>
+        <v>11.81175051977283</v>
       </c>
       <c r="M87" t="n">
-        <v>1.646421662111117e-25</v>
+        <v>5.885497453460582e-26</v>
       </c>
       <c r="N87" t="n">
-        <v>1.692446229136148e-12</v>
+        <v>1.02921435692802e-12</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -4984,7 +4984,7 @@
         </is>
       </c>
       <c r="P87" t="n">
-        <v>0.0003176999999965346</v>
+        <v>0.000331499999999707</v>
       </c>
     </row>
     <row r="88">
@@ -5004,13 +5004,13 @@
         <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>10.00000000000003</v>
+        <v>10.00000000000013</v>
       </c>
       <c r="G88" t="n">
-        <v>36.46925165320068</v>
+        <v>36.46925165320037</v>
       </c>
       <c r="H88" t="n">
-        <v>5.485117248731578</v>
+        <v>5.485117248731877</v>
       </c>
       <c r="I88" t="n">
         <v>21.84848718910419</v>
@@ -5019,16 +5019,16 @@
         <v>13.65786460130007</v>
       </c>
       <c r="K88" t="n">
-        <v>21.8484871891042</v>
+        <v>21.84848718910428</v>
       </c>
       <c r="L88" t="n">
-        <v>13.65786460130069</v>
+        <v>13.65786460130114</v>
       </c>
       <c r="M88" t="n">
-        <v>8.949145827821165e-28</v>
+        <v>2.739413522738396e-27</v>
       </c>
       <c r="N88" t="n">
-        <v>1.309388437956397e-13</v>
+        <v>2.446206259061489e-13</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -5036,7 +5036,7 @@
         </is>
       </c>
       <c r="P88" t="n">
-        <v>0.0004263000000008788</v>
+        <v>0.0002019000000004212</v>
       </c>
     </row>
     <row r="89">
@@ -5056,13 +5056,13 @@
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>9.999999999983569</v>
+        <v>10.00000000000356</v>
       </c>
       <c r="G89" t="n">
-        <v>118.1275533419261</v>
+        <v>118.1275533419336</v>
       </c>
       <c r="H89" t="n">
-        <v>14.45881652292921</v>
+        <v>14.45881652296511</v>
       </c>
       <c r="I89" t="n">
         <v>92.7668218217183</v>
@@ -5071,16 +5071,16 @@
         <v>16.49115940110462</v>
       </c>
       <c r="K89" t="n">
-        <v>92.76682182171682</v>
+        <v>92.76682182171859</v>
       </c>
       <c r="L89" t="n">
-        <v>16.49115940107399</v>
+        <v>16.49115940111098</v>
       </c>
       <c r="M89" t="n">
-        <v>2.529463773706854e-24</v>
+        <v>1.169689397975134e-25</v>
       </c>
       <c r="N89" t="n">
-        <v>8.722115529062005e-12</v>
+        <v>1.849781297617242e-12</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
         </is>
       </c>
       <c r="P89" t="n">
-        <v>0.0002979000000067344</v>
+        <v>0.0001932000000000045</v>
       </c>
     </row>
     <row r="90">
@@ -5108,13 +5108,13 @@
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>10.00000000000215</v>
+        <v>10.00000000000171</v>
       </c>
       <c r="G90" t="n">
         <v>116.5591888835452</v>
       </c>
       <c r="H90" t="n">
-        <v>9.085796258559681</v>
+        <v>9.08579625855911</v>
       </c>
       <c r="I90" t="n">
         <v>77.06502614626034</v>
@@ -5123,16 +5123,16 @@
         <v>11.20723949811577</v>
       </c>
       <c r="K90" t="n">
-        <v>77.06502614626096</v>
+        <v>77.06502614626091</v>
       </c>
       <c r="L90" t="n">
-        <v>11.20723949811855</v>
+        <v>11.20723949811793</v>
       </c>
       <c r="M90" t="n">
-        <v>1.04889790191271e-25</v>
+        <v>6.477937370683945e-26</v>
       </c>
       <c r="N90" t="n">
-        <v>1.342476536445409e-12</v>
+        <v>1.078118215840345e-12</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -5140,7 +5140,7 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>0.0003138000000006969</v>
+        <v>0.0001959000000013589</v>
       </c>
     </row>
     <row r="91">
@@ -5160,13 +5160,13 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>9.999999999999622</v>
+        <v>10.00000000000069</v>
       </c>
       <c r="G91" t="n">
-        <v>89.94497768438961</v>
+        <v>89.94497768439122</v>
       </c>
       <c r="H91" t="n">
-        <v>6.071245611739692</v>
+        <v>6.071245611740673</v>
       </c>
       <c r="I91" t="n">
         <v>48.84601329812367</v>
@@ -5175,16 +5175,16 @@
         <v>11.23051578470421</v>
       </c>
       <c r="K91" t="n">
-        <v>48.84601329812346</v>
+        <v>48.84601329812407</v>
       </c>
       <c r="L91" t="n">
-        <v>11.2305157847031</v>
+        <v>11.23051578470456</v>
       </c>
       <c r="M91" t="n">
-        <v>7.218160729767584e-27</v>
+        <v>2.376243288688967e-26</v>
       </c>
       <c r="N91" t="n">
-        <v>3.717545646572836e-13</v>
+        <v>4.378156327986766e-13</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -5192,7 +5192,7 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>0.0003001999999980853</v>
+        <v>0.0001896999999999593</v>
       </c>
     </row>
     <row r="92">
@@ -5212,13 +5212,13 @@
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>10.00000000000002</v>
+        <v>10.00000000000005</v>
       </c>
       <c r="G92" t="n">
-        <v>27.54975577790645</v>
+        <v>27.54975577790663</v>
       </c>
       <c r="H92" t="n">
-        <v>4.892227932112924</v>
+        <v>4.89222793211289</v>
       </c>
       <c r="I92" t="n">
         <v>17.15395993153109</v>
@@ -5227,16 +5227,16 @@
         <v>13.17470023696191</v>
       </c>
       <c r="K92" t="n">
-        <v>17.15395993153111</v>
+        <v>17.15395993153112</v>
       </c>
       <c r="L92" t="n">
-        <v>13.17470023696127</v>
+        <v>13.17470023696126</v>
       </c>
       <c r="M92" t="n">
-        <v>1.230743196904686e-28</v>
+        <v>1.478507691686374e-28</v>
       </c>
       <c r="N92" t="n">
-        <v>9.92825870905289e-14</v>
+        <v>9.636185344775768e-14</v>
       </c>
       <c r="O92" t="inlineStr">
         <is>
@@ -5244,7 +5244,7 @@
         </is>
       </c>
       <c r="P92" t="n">
-        <v>0.0002968000000009852</v>
+        <v>0.000234400000000079</v>
       </c>
     </row>
     <row r="93">
@@ -5264,13 +5264,13 @@
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>9.999999999999671</v>
+        <v>10.00000000000025</v>
       </c>
       <c r="G93" t="n">
-        <v>36.18064730123466</v>
+        <v>36.18064730123607</v>
       </c>
       <c r="H93" t="n">
-        <v>6.948245597905843</v>
+        <v>6.948245597906274</v>
       </c>
       <c r="I93" t="n">
         <v>23.34892049549794</v>
@@ -5279,16 +5279,16 @@
         <v>15.37253312835461</v>
       </c>
       <c r="K93" t="n">
-        <v>23.34892049549774</v>
+        <v>23.34892049549807</v>
       </c>
       <c r="L93" t="n">
-        <v>15.37253312835408</v>
+        <v>15.37253312835506</v>
       </c>
       <c r="M93" t="n">
-        <v>7.074214944484093e-27</v>
+        <v>2.720831185629769e-27</v>
       </c>
       <c r="N93" t="n">
-        <v>2.46445082175294e-13</v>
+        <v>1.293128592815035e-13</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -5296,7 +5296,7 @@
         </is>
       </c>
       <c r="P93" t="n">
-        <v>0.0003257999999988215</v>
+        <v>0.0001995000000007963</v>
       </c>
     </row>
     <row r="94">
@@ -5316,13 +5316,13 @@
         <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>10.00000000000085</v>
+        <v>10.00000000000239</v>
       </c>
       <c r="G94" t="n">
-        <v>159.4584898987723</v>
+        <v>159.4584898987716</v>
       </c>
       <c r="H94" t="n">
-        <v>12.462978801646</v>
+        <v>12.4629788016484</v>
       </c>
       <c r="I94" t="n">
         <v>135.8914103371119</v>
@@ -5331,16 +5331,16 @@
         <v>9.221215218233809</v>
       </c>
       <c r="K94" t="n">
-        <v>135.8914103371116</v>
+        <v>135.8914103371111</v>
       </c>
       <c r="L94" t="n">
-        <v>9.221215218234727</v>
+        <v>9.221215218236329</v>
       </c>
       <c r="M94" t="n">
-        <v>4.505022918142855e-26</v>
+        <v>3.425501388763254e-25</v>
       </c>
       <c r="N94" t="n">
-        <v>5.145761167161674e-13</v>
+        <v>1.431946590529992e-12</v>
       </c>
       <c r="O94" t="inlineStr">
         <is>
@@ -5348,7 +5348,7 @@
         </is>
       </c>
       <c r="P94" t="n">
-        <v>0.0003545999999943206</v>
+        <v>0.0001829999999998222</v>
       </c>
     </row>
     <row r="95">
@@ -5368,13 +5368,13 @@
         <v>0</v>
       </c>
       <c r="F95" t="n">
-        <v>10.00000000000438</v>
+        <v>9.999999999991216</v>
       </c>
       <c r="G95" t="n">
-        <v>109.1437807997684</v>
+        <v>109.1437807997599</v>
       </c>
       <c r="H95" t="n">
-        <v>10.89013882342007</v>
+        <v>10.89013882340123</v>
       </c>
       <c r="I95" t="n">
         <v>77.08991880558148</v>
@@ -5383,16 +5383,16 @@
         <v>13.86645042167153</v>
       </c>
       <c r="K95" t="n">
-        <v>77.08991880558257</v>
+        <v>77.08991880557922</v>
       </c>
       <c r="L95" t="n">
-        <v>13.86645042167823</v>
+        <v>13.86645042165716</v>
       </c>
       <c r="M95" t="n">
-        <v>3.213878743084232e-25</v>
+        <v>1.278154679283223e-24</v>
       </c>
       <c r="N95" t="n">
-        <v>2.585694307852714e-12</v>
+        <v>5.323774532257818e-12</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -5400,7 +5400,7 @@
         </is>
       </c>
       <c r="P95" t="n">
-        <v>0.0002891000000033728</v>
+        <v>0.0001857999999987925</v>
       </c>
     </row>
     <row r="96">
@@ -5420,13 +5420,13 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>9.999999999998462</v>
+        <v>9.999999999993564</v>
       </c>
       <c r="G96" t="n">
-        <v>129.4894415239123</v>
+        <v>129.4894415239114</v>
       </c>
       <c r="H96" t="n">
-        <v>10.28665410746174</v>
+        <v>10.28665410745497</v>
       </c>
       <c r="I96" t="n">
         <v>92.4963307677606</v>
@@ -5435,16 +5435,16 @@
         <v>10.70698393477249</v>
       </c>
       <c r="K96" t="n">
-        <v>92.49633076776034</v>
+        <v>92.49633076775953</v>
       </c>
       <c r="L96" t="n">
-        <v>10.7069839347706</v>
+        <v>10.70698393476444</v>
       </c>
       <c r="M96" t="n">
-        <v>3.557506715683096e-26</v>
+        <v>6.14075712217521e-25</v>
       </c>
       <c r="N96" t="n">
-        <v>8.834688794049207e-13</v>
+        <v>3.715479595755251e-12</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -5452,7 +5452,7 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>0.0003394999999954962</v>
+        <v>0.0001883999999989783</v>
       </c>
     </row>
     <row r="97">
@@ -5472,13 +5472,13 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>10.00000000000001</v>
+        <v>9.999999999999881</v>
       </c>
       <c r="G97" t="n">
-        <v>41.18462776024207</v>
+        <v>41.18462776024172</v>
       </c>
       <c r="H97" t="n">
-        <v>5.288256223490247</v>
+        <v>5.288256223490152</v>
       </c>
       <c r="I97" t="n">
         <v>23.74542453059524</v>
@@ -5487,16 +5487,16 @@
         <v>13.28409758323217</v>
       </c>
       <c r="K97" t="n">
-        <v>23.74542453059525</v>
+        <v>23.74542453059517</v>
       </c>
       <c r="L97" t="n">
-        <v>13.28409758323314</v>
+        <v>13.28409758323293</v>
       </c>
       <c r="M97" t="n">
-        <v>2.491110409489791e-28</v>
+        <v>8.09812865009276e-28</v>
       </c>
       <c r="N97" t="n">
-        <v>1.507059352605675e-13</v>
+        <v>1.504714130962823e-13</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -5504,7 +5504,7 @@
         </is>
       </c>
       <c r="P97" t="n">
-        <v>0.0003123999999985472</v>
+        <v>0.0002389000000011521</v>
       </c>
     </row>
     <row r="98">
@@ -5524,13 +5524,13 @@
         <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>10.00000000000058</v>
+        <v>10.00000000000057</v>
       </c>
       <c r="G98" t="n">
-        <v>38.64364002302929</v>
+        <v>38.64364002302933</v>
       </c>
       <c r="H98" t="n">
-        <v>13.91402845610114</v>
+        <v>13.91402845610106</v>
       </c>
       <c r="I98" t="n">
         <v>29.58813609103335</v>
@@ -5542,13 +5542,13 @@
         <v>29.58813609103354</v>
       </c>
       <c r="L98" t="n">
-        <v>23.48744640074259</v>
+        <v>23.48744640074248</v>
       </c>
       <c r="M98" t="n">
-        <v>1.703677141780905e-26</v>
+        <v>1.399600086283076e-26</v>
       </c>
       <c r="N98" t="n">
-        <v>4.512436252496143e-13</v>
+        <v>4.284999027256134e-13</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -5556,7 +5556,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>0.0002945999999894866</v>
+        <v>0.0001964000000000965</v>
       </c>
     </row>
     <row r="99">
@@ -5576,13 +5576,13 @@
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>10.00000000000219</v>
+        <v>10.0000000000006</v>
       </c>
       <c r="G99" t="n">
-        <v>150.6499423676138</v>
+        <v>150.6499423676141</v>
       </c>
       <c r="H99" t="n">
-        <v>14.64283022328786</v>
+        <v>14.64283022328503</v>
       </c>
       <c r="I99" t="n">
         <v>129.036147186146</v>
@@ -5591,16 +5591,16 @@
         <v>12.59476915243944</v>
       </c>
       <c r="K99" t="n">
-        <v>129.0361471861456</v>
+        <v>129.0361471861459</v>
       </c>
       <c r="L99" t="n">
-        <v>12.59476915244238</v>
+        <v>12.5947691524402</v>
       </c>
       <c r="M99" t="n">
-        <v>1.972151738614699e-25</v>
+        <v>1.410996767945608e-26</v>
       </c>
       <c r="N99" t="n">
-        <v>1.18042755729956e-12</v>
+        <v>3.225662904150851e-13</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -5608,7 +5608,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>0.001026199999998312</v>
+        <v>0.0001920999999995843</v>
       </c>
     </row>
     <row r="100">
@@ -5628,13 +5628,13 @@
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>10.00000000001037</v>
+        <v>9.999999999988384</v>
       </c>
       <c r="G100" t="n">
-        <v>131.8081046523943</v>
+        <v>131.8081046523922</v>
       </c>
       <c r="H100" t="n">
-        <v>9.806268185424488</v>
+        <v>9.806268185395085</v>
       </c>
       <c r="I100" t="n">
         <v>92.65513206400841</v>
@@ -5643,16 +5643,16 @@
         <v>9.952434050938109</v>
       </c>
       <c r="K100" t="n">
-        <v>92.65513206401013</v>
+        <v>92.65513206400648</v>
       </c>
       <c r="L100" t="n">
-        <v>9.952434050950195</v>
+        <v>9.95243405092412</v>
       </c>
       <c r="M100" t="n">
-        <v>1.73309310687415e-24</v>
+        <v>2.169577150549488e-24</v>
       </c>
       <c r="N100" t="n">
-        <v>6.010193669031283e-12</v>
+        <v>6.814290221169022e-12</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -5660,7 +5660,7 @@
         </is>
       </c>
       <c r="P100" t="n">
-        <v>0.0003911999999957061</v>
+        <v>0.0002316999999987246</v>
       </c>
     </row>
     <row r="101">
@@ -5680,13 +5680,13 @@
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>9.999999999997371</v>
+        <v>10.0000000000036</v>
       </c>
       <c r="G101" t="n">
-        <v>121.0101405535415</v>
+        <v>121.0101405535437</v>
       </c>
       <c r="H101" t="n">
-        <v>8.856940790883742</v>
+        <v>8.856940790891493</v>
       </c>
       <c r="I101" t="n">
         <v>79.48494662297404</v>
@@ -5695,16 +5695,16 @@
         <v>10.4553174329922</v>
       </c>
       <c r="K101" t="n">
-        <v>79.48494662297321</v>
+        <v>79.48494662297509</v>
       </c>
       <c r="L101" t="n">
-        <v>10.45531743298878</v>
+        <v>10.45531743299662</v>
       </c>
       <c r="M101" t="n">
-        <v>1.565635161929202e-25</v>
+        <v>2.98549555016362e-25</v>
       </c>
       <c r="N101" t="n">
-        <v>1.696670717527305e-12</v>
+        <v>2.26210006072457e-12</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -5712,7 +5712,7 @@
         </is>
       </c>
       <c r="P101" t="n">
-        <v>0.0003001999999980853</v>
+        <v>0.0002164000000011157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>